<commit_message>
Add predict sell price
</commit_message>
<xml_diff>
--- a/Data/binance_ETHUSDT_data.xlsx
+++ b/Data/binance_ETHUSDT_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X73"/>
+  <dimension ref="A1:X74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6936,12 +6936,12 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>161.91000000</t>
+          <t>158.59000000</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>631043.09258000</t>
+          <t>809100.24594000</t>
         </is>
       </c>
       <c r="G73" t="n">
@@ -6949,20 +6949,20 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>101043805.88741570</t>
+          <t>129919934.44376530</t>
         </is>
       </c>
       <c r="I73" t="n">
-        <v>172218</v>
+        <v>223429</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>305971.54188000</t>
+          <t>396232.44593000</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>48979881.19648620</t>
+          <t>63624893.23050370</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
@@ -6971,40 +6971,132 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>161.9099999999999</v>
+        <v>158.5899999999998</v>
       </c>
       <c r="N73" t="n">
-        <v>160.12</v>
+        <v>158.4600000000001</v>
       </c>
       <c r="O73" t="n">
-        <v>165.2328571428571</v>
+        <v>164.7585714285714</v>
       </c>
       <c r="P73" t="n">
-        <v>150.0646666666667</v>
+        <v>149.8433333333334</v>
       </c>
       <c r="Q73" t="n">
-        <v>139.2666666666667</v>
+        <v>139.1560000000001</v>
       </c>
       <c r="R73" t="n">
-        <v>161.91</v>
+        <v>158.59</v>
       </c>
       <c r="S73" t="n">
-        <v>161.0981333966001</v>
+        <v>158.8848000632668</v>
       </c>
       <c r="T73" t="n">
-        <v>155.9607387807031</v>
+        <v>155.4499664979708</v>
       </c>
       <c r="U73" t="n">
-        <v>154.4607103875306</v>
+        <v>154.2138161826309</v>
       </c>
       <c r="V73" t="n">
-        <v>1.500028393172556</v>
+        <v>1.236150315339898</v>
       </c>
       <c r="W73" t="n">
-        <v>-2.911044003508873</v>
+        <v>-2.963819624633326</v>
       </c>
       <c r="X73" t="n">
-        <v>4.41107239668143</v>
+        <v>4.199969939973224</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>158.56000000</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>158.57000000</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>150.00000000</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>153.16000000</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>784119.92972000</t>
+        </is>
+      </c>
+      <c r="G74" t="n">
+        <v>1586822399999</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>120207813.31358490</t>
+        </is>
+      </c>
+      <c r="I74" t="n">
+        <v>183811</v>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>383660.81768000</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>58830933.96878600</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>2020-04-13 08:00:00</t>
+        </is>
+      </c>
+      <c r="M74" t="n">
+        <v>153.1599999999998</v>
+      </c>
+      <c r="N74" t="n">
+        <v>155.8750000000001</v>
+      </c>
+      <c r="O74" t="n">
+        <v>162.1642857142857</v>
+      </c>
+      <c r="P74" t="n">
+        <v>151.754</v>
+      </c>
+      <c r="Q74" t="n">
+        <v>140.1766666666667</v>
+      </c>
+      <c r="R74" t="n">
+        <v>153.16</v>
+      </c>
+      <c r="S74" t="n">
+        <v>155.0682666877556</v>
+      </c>
+      <c r="T74" t="n">
+        <v>155.0976621785944</v>
+      </c>
+      <c r="U74" t="n">
+        <v>154.1354712281884</v>
+      </c>
+      <c r="V74" t="n">
+        <v>0.9621909504060397</v>
+      </c>
+      <c r="W74" t="n">
+        <v>-2.1786174434723</v>
+      </c>
+      <c r="X74" t="n">
+        <v>3.14080839387834</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the log with zip
</commit_message>
<xml_diff>
--- a/Data/binance_ETHUSDT_data.xlsx
+++ b/Data/binance_ETHUSDT_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X74"/>
+  <dimension ref="A1:X83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7018,7 +7018,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>158.57000000</t>
+          <t>158.97000000</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -7028,12 +7028,12 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>153.16000000</t>
+          <t>156.29000000</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>784119.92972000</t>
+          <t>1042091.03622000</t>
         </is>
       </c>
       <c r="G74" t="n">
@@ -7041,20 +7041,20 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>120207813.31358490</t>
+          <t>160423270.30371500</t>
         </is>
       </c>
       <c r="I74" t="n">
-        <v>183811</v>
+        <v>255965</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>383660.81768000</t>
+          <t>519763.88357000</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>58830933.96878600</t>
+          <t>80051376.52875040</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
@@ -7063,40 +7063,868 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>153.1599999999998</v>
+        <v>156.2899999999998</v>
       </c>
       <c r="N74" t="n">
-        <v>155.8750000000001</v>
+        <v>157.4400000000001</v>
       </c>
       <c r="O74" t="n">
-        <v>162.1642857142857</v>
+        <v>162.6114285714285</v>
       </c>
       <c r="P74" t="n">
-        <v>151.754</v>
+        <v>151.9626666666667</v>
       </c>
       <c r="Q74" t="n">
-        <v>140.1766666666667</v>
+        <v>140.2810000000001</v>
       </c>
       <c r="R74" t="n">
-        <v>153.16</v>
+        <v>156.29</v>
       </c>
       <c r="S74" t="n">
-        <v>155.0682666877556</v>
+        <v>157.1549333544223</v>
       </c>
       <c r="T74" t="n">
-        <v>155.0976621785944</v>
+        <v>155.5792030747713</v>
       </c>
       <c r="U74" t="n">
-        <v>154.1354712281884</v>
+        <v>154.3681680793534</v>
       </c>
       <c r="V74" t="n">
-        <v>0.9621909504060397</v>
+        <v>1.211034995417947</v>
       </c>
       <c r="W74" t="n">
-        <v>-2.1786174434723</v>
+        <v>-2.128848630276904</v>
       </c>
       <c r="X74" t="n">
-        <v>3.14080839387834</v>
+        <v>3.339883625694851</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>156.28000000</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>161.85000000</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>155.23000000</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>158.45000000</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>698030.65089000</t>
+        </is>
+      </c>
+      <c r="G75" t="n">
+        <v>1586908799999</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>110710086.10400900</t>
+        </is>
+      </c>
+      <c r="I75" t="n">
+        <v>178490</v>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>343955.51426000</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>54564372.10918630</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>2020-04-14 08:00:00</t>
+        </is>
+      </c>
+      <c r="M75" t="n">
+        <v>158.4499999999998</v>
+      </c>
+      <c r="N75" t="n">
+        <v>157.3700000000001</v>
+      </c>
+      <c r="O75" t="n">
+        <v>161.7285714285714</v>
+      </c>
+      <c r="P75" t="n">
+        <v>153.7220000000001</v>
+      </c>
+      <c r="Q75" t="n">
+        <v>141.4366666666668</v>
+      </c>
+      <c r="R75" t="n">
+        <v>158.45</v>
+      </c>
+      <c r="S75" t="n">
+        <v>158.0183111181408</v>
+      </c>
+      <c r="T75" t="n">
+        <v>156.0208660296681</v>
+      </c>
+      <c r="U75" t="n">
+        <v>154.6715460604184</v>
+      </c>
+      <c r="V75" t="n">
+        <v>1.349319969249649</v>
+      </c>
+      <c r="W75" t="n">
+        <v>-1.43321486348597</v>
+      </c>
+      <c r="X75" t="n">
+        <v>2.782534832735619</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>158.46000000</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>161.29000000</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>152.00000000</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>152.73000000</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>729119.66505000</t>
+        </is>
+      </c>
+      <c r="G76" t="n">
+        <v>1586995199999</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>114640840.11551650</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>186226</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>347034.48291000</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>54594699.03576640</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>2020-04-15 08:00:00</t>
+        </is>
+      </c>
+      <c r="M76" t="n">
+        <v>152.7299999999998</v>
+      </c>
+      <c r="N76" t="n">
+        <v>155.5900000000001</v>
+      </c>
+      <c r="O76" t="n">
+        <v>158.8171428571428</v>
+      </c>
+      <c r="P76" t="n">
+        <v>155.0560000000001</v>
+      </c>
+      <c r="Q76" t="n">
+        <v>142.8270000000001</v>
+      </c>
+      <c r="R76" t="n">
+        <v>152.73</v>
+      </c>
+      <c r="S76" t="n">
+        <v>154.4927703727136</v>
+      </c>
+      <c r="T76" t="n">
+        <v>155.5145771154511</v>
+      </c>
+      <c r="U76" t="n">
+        <v>154.527278688836</v>
+      </c>
+      <c r="V76" t="n">
+        <v>0.9872984266150979</v>
+      </c>
+      <c r="W76" t="n">
+        <v>-0.9491121793629917</v>
+      </c>
+      <c r="X76" t="n">
+        <v>1.93641060597809</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>152.74000000</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>174.79000000</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>148.33000000</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>172.29000000</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>1647207.59991000</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>1587081599999</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>273639160.06938750</t>
+        </is>
+      </c>
+      <c r="I77" t="n">
+        <v>389854</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>830355.78324000</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>137897793.15056740</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>2020-04-16 08:00:00</t>
+        </is>
+      </c>
+      <c r="M77" t="n">
+        <v>172.2899999999998</v>
+      </c>
+      <c r="N77" t="n">
+        <v>162.5100000000001</v>
+      </c>
+      <c r="O77" t="n">
+        <v>159.2128571428571</v>
+      </c>
+      <c r="P77" t="n">
+        <v>157.4960000000001</v>
+      </c>
+      <c r="Q77" t="n">
+        <v>144.7143333333334</v>
+      </c>
+      <c r="R77" t="n">
+        <v>172.29</v>
+      </c>
+      <c r="S77" t="n">
+        <v>166.3575901242378</v>
+      </c>
+      <c r="T77" t="n">
+        <v>158.0954193105433</v>
+      </c>
+      <c r="U77" t="n">
+        <v>155.84683967885</v>
+      </c>
+      <c r="V77" t="n">
+        <v>2.248579631693275</v>
+      </c>
+      <c r="W77" t="n">
+        <v>-0.3095737895646652</v>
+      </c>
+      <c r="X77" t="n">
+        <v>2.55815342125794</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>172.31000000</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>174.96000000</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>168.31000000</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>170.69000000</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>723537.75591000</t>
+        </is>
+      </c>
+      <c r="G78" t="n">
+        <v>1587167999999</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>123553456.31967860</t>
+        </is>
+      </c>
+      <c r="I78" t="n">
+        <v>191289</v>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>352005.34180000</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>60121889.86467380</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>2020-04-17 08:00:00</t>
+        </is>
+      </c>
+      <c r="M78" t="n">
+        <v>170.6899999999998</v>
+      </c>
+      <c r="N78" t="n">
+        <v>171.4900000000001</v>
+      </c>
+      <c r="O78" t="n">
+        <v>161.0528571428571</v>
+      </c>
+      <c r="P78" t="n">
+        <v>159.4566666666667</v>
+      </c>
+      <c r="Q78" t="n">
+        <v>146.467</v>
+      </c>
+      <c r="R78" t="n">
+        <v>170.69</v>
+      </c>
+      <c r="S78" t="n">
+        <v>169.2458633747459</v>
+      </c>
+      <c r="T78" t="n">
+        <v>160.0330521308449</v>
+      </c>
+      <c r="U78" t="n">
+        <v>156.9492755881899</v>
+      </c>
+      <c r="V78" t="n">
+        <v>3.083776542655016</v>
+      </c>
+      <c r="W78" t="n">
+        <v>0.369096300299315</v>
+      </c>
+      <c r="X78" t="n">
+        <v>2.714680242355701</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>170.61000000</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>189.54000000</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>170.48000000</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>187.40000000</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>1127296.36979000</t>
+        </is>
+      </c>
+      <c r="G79" t="n">
+        <v>1587254399999</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>203132211.95640910</t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>286172</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>569708.87703000</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>102696714.57128610</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>2020-04-18 08:00:00</t>
+        </is>
+      </c>
+      <c r="M79" t="n">
+        <v>187.3999999999998</v>
+      </c>
+      <c r="N79" t="n">
+        <v>179.0450000000001</v>
+      </c>
+      <c r="O79" t="n">
+        <v>165.2057142857143</v>
+      </c>
+      <c r="P79" t="n">
+        <v>162.5293333333334</v>
+      </c>
+      <c r="Q79" t="n">
+        <v>148.1703333333334</v>
+      </c>
+      <c r="R79" t="n">
+        <v>187.4</v>
+      </c>
+      <c r="S79" t="n">
+        <v>181.3486211249153</v>
+      </c>
+      <c r="T79" t="n">
+        <v>164.2433610364284</v>
+      </c>
+      <c r="U79" t="n">
+        <v>159.2104731794591</v>
+      </c>
+      <c r="V79" t="n">
+        <v>5.032887856969325</v>
+      </c>
+      <c r="W79" t="n">
+        <v>1.301854637383962</v>
+      </c>
+      <c r="X79" t="n">
+        <v>3.731033219585362</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>187.40000000</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>188.35000000</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>175.75000000</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>180.03000000</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>995759.57750000</t>
+        </is>
+      </c>
+      <c r="G80" t="n">
+        <v>1587340799999</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>181415813.50269480</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
+        <v>270668</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>478833.69271000</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>87227250.30026600</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>2020-04-19 08:00:00</t>
+        </is>
+      </c>
+      <c r="M80" t="n">
+        <v>180.0299999999998</v>
+      </c>
+      <c r="N80" t="n">
+        <v>183.7150000000001</v>
+      </c>
+      <c r="O80" t="n">
+        <v>168.2685714285714</v>
+      </c>
+      <c r="P80" t="n">
+        <v>164.9246666666668</v>
+      </c>
+      <c r="Q80" t="n">
+        <v>149.722</v>
+      </c>
+      <c r="R80" t="n">
+        <v>180.03</v>
+      </c>
+      <c r="S80" t="n">
+        <v>180.4695403749718</v>
+      </c>
+      <c r="T80" t="n">
+        <v>166.6720792299954</v>
+      </c>
+      <c r="U80" t="n">
+        <v>160.7561975166961</v>
+      </c>
+      <c r="V80" t="n">
+        <v>5.915881713299285</v>
+      </c>
+      <c r="W80" t="n">
+        <v>2.224660072947727</v>
+      </c>
+      <c r="X80" t="n">
+        <v>3.691221640351558</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>180.02000000</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>186.46000000</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>166.70000000</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>170.20000000</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>1547821.52737000</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
+        <v>1587427199999</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>273854539.80380100</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>365589</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>745586.67414000</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>131918687.66076710</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>2020-04-20 08:00:00</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>170.1999999999998</v>
+      </c>
+      <c r="N81" t="n">
+        <v>175.1150000000001</v>
+      </c>
+      <c r="O81" t="n">
+        <v>170.2557142857143</v>
+      </c>
+      <c r="P81" t="n">
+        <v>166.7593333333334</v>
+      </c>
+      <c r="Q81" t="n">
+        <v>150.9733333333334</v>
+      </c>
+      <c r="R81" t="n">
+        <v>170.2</v>
+      </c>
+      <c r="S81" t="n">
+        <v>173.6231801249906</v>
+      </c>
+      <c r="T81" t="n">
+        <v>167.2148371237567</v>
+      </c>
+      <c r="U81" t="n">
+        <v>161.4572238087152</v>
+      </c>
+      <c r="V81" t="n">
+        <v>5.757613315041425</v>
+      </c>
+      <c r="W81" t="n">
+        <v>2.931250733850843</v>
+      </c>
+      <c r="X81" t="n">
+        <v>2.826362581190582</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>170.21000000</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>174.70000000</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>168.00000000</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>170.74000000</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>906381.65398000</t>
+        </is>
+      </c>
+      <c r="G82" t="n">
+        <v>1587513599999</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>155292048.43579020</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>228262</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>454400.78888000</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>77856857.48694720</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>2020-04-21 08:00:00</t>
+        </is>
+      </c>
+      <c r="M82" t="n">
+        <v>170.7399999999998</v>
+      </c>
+      <c r="N82" t="n">
+        <v>170.4700000000001</v>
+      </c>
+      <c r="O82" t="n">
+        <v>172.0114285714286</v>
+      </c>
+      <c r="P82" t="n">
+        <v>166.7206666666667</v>
+      </c>
+      <c r="Q82" t="n">
+        <v>152.5873333333334</v>
+      </c>
+      <c r="R82" t="n">
+        <v>170.74</v>
+      </c>
+      <c r="S82" t="n">
+        <v>171.7010600416635</v>
+      </c>
+      <c r="T82" t="n">
+        <v>167.7571705944951</v>
+      </c>
+      <c r="U82" t="n">
+        <v>162.1461885365169</v>
+      </c>
+      <c r="V82" t="n">
+        <v>5.610982057978191</v>
+      </c>
+      <c r="W82" t="n">
+        <v>3.467197006251793</v>
+      </c>
+      <c r="X82" t="n">
+        <v>2.143785051726398</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>170.73000000</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>184.00000000</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>169.78000000</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>181.38000000</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>812086.87602000</t>
+        </is>
+      </c>
+      <c r="G83" t="n">
+        <v>1587599999999</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>143959338.71980660</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
+        <v>196518</v>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>399591.00926000</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>70844470.39062520</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>2020-04-22 08:00:00</t>
+        </is>
+      </c>
+      <c r="M83" t="n">
+        <v>181.3799999999998</v>
+      </c>
+      <c r="N83" t="n">
+        <v>176.0600000000001</v>
+      </c>
+      <c r="O83" t="n">
+        <v>176.1042857142857</v>
+      </c>
+      <c r="P83" t="n">
+        <v>167.8373333333334</v>
+      </c>
+      <c r="Q83" t="n">
+        <v>154.1026666666667</v>
+      </c>
+      <c r="R83" t="n">
+        <v>181.38</v>
+      </c>
+      <c r="S83" t="n">
+        <v>178.1536866805545</v>
+      </c>
+      <c r="T83" t="n">
+        <v>169.8529928591669</v>
+      </c>
+      <c r="U83" t="n">
+        <v>163.5735081370333</v>
+      </c>
+      <c r="V83" t="n">
+        <v>6.279484722133674</v>
+      </c>
+      <c r="W83" t="n">
+        <v>4.029654555788338</v>
+      </c>
+      <c r="X83" t="n">
+        <v>2.249830166345336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust the alert condition
</commit_message>
<xml_diff>
--- a/Data/binance_ETHUSDT_data.xlsx
+++ b/Data/binance_ETHUSDT_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X83"/>
+  <dimension ref="A1:X132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7856,12 +7856,12 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>181.38000000</t>
+          <t>182.70000000</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>812086.87602000</t>
+          <t>988698.39076000</t>
         </is>
       </c>
       <c r="G83" t="n">
@@ -7869,20 +7869,20 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>143959338.71980660</t>
+          <t>176079076.92749950</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>196518</v>
+        <v>246896</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>399591.00926000</t>
+          <t>488185.26353000</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>70844470.39062520</t>
+          <t>86960811.93958360</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
@@ -7891,40 +7891,4548 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>181.3799999999998</v>
+        <v>182.6999999999998</v>
       </c>
       <c r="N83" t="n">
-        <v>176.0600000000001</v>
+        <v>176.7200000000001</v>
       </c>
       <c r="O83" t="n">
-        <v>176.1042857142857</v>
+        <v>176.2928571428572</v>
       </c>
       <c r="P83" t="n">
-        <v>167.8373333333334</v>
+        <v>167.9253333333334</v>
       </c>
       <c r="Q83" t="n">
-        <v>154.1026666666667</v>
+        <v>154.1466666666667</v>
       </c>
       <c r="R83" t="n">
-        <v>181.38</v>
+        <v>182.7</v>
       </c>
       <c r="S83" t="n">
-        <v>178.1536866805545</v>
+        <v>179.0336866805545</v>
       </c>
       <c r="T83" t="n">
-        <v>169.8529928591669</v>
+        <v>170.0560700105441</v>
       </c>
       <c r="U83" t="n">
-        <v>163.5735081370333</v>
+        <v>163.6714638581995</v>
       </c>
       <c r="V83" t="n">
-        <v>6.279484722133674</v>
+        <v>6.384606152344617</v>
       </c>
       <c r="W83" t="n">
-        <v>4.029654555788338</v>
+        <v>4.050678842068265</v>
       </c>
       <c r="X83" t="n">
-        <v>2.249830166345336</v>
+        <v>2.333927310276351</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>182.70000000</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>193.63000000</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>178.16000000</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>185.51000000</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>1457867.08713000</t>
+        </is>
+      </c>
+      <c r="G84" t="n">
+        <v>1587686399999</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>270862911.36856540</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>363772</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>719694.31692000</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>133791885.01731330</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>2020-04-23 08:00:00</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>185.5099999999998</v>
+      </c>
+      <c r="N84" t="n">
+        <v>184.105</v>
+      </c>
+      <c r="O84" t="n">
+        <v>178.1814285714286</v>
+      </c>
+      <c r="P84" t="n">
+        <v>168.752</v>
+      </c>
+      <c r="Q84" t="n">
+        <v>155.7163333333334</v>
+      </c>
+      <c r="R84" t="n">
+        <v>185.51</v>
+      </c>
+      <c r="S84" t="n">
+        <v>183.3512288935182</v>
+      </c>
+      <c r="T84" t="n">
+        <v>172.4335999628548</v>
+      </c>
+      <c r="U84" t="n">
+        <v>165.291858720649</v>
+      </c>
+      <c r="V84" t="n">
+        <v>7.141741242205796</v>
+      </c>
+      <c r="W84" t="n">
+        <v>4.66889132768828</v>
+      </c>
+      <c r="X84" t="n">
+        <v>2.472849914517516</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>185.57000000</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>189.80000000</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>184.72000000</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>187.59000000</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>780904.21257000</t>
+        </is>
+      </c>
+      <c r="G85" t="n">
+        <v>1587772799999</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>146419748.08164820</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>222074</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>368634.10604000</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>69133236.24006010</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>2020-04-24 08:00:00</t>
+        </is>
+      </c>
+      <c r="M85" t="n">
+        <v>187.5899999999998</v>
+      </c>
+      <c r="N85" t="n">
+        <v>186.55</v>
+      </c>
+      <c r="O85" t="n">
+        <v>180.5957142857143</v>
+      </c>
+      <c r="P85" t="n">
+        <v>169.9566666666667</v>
+      </c>
+      <c r="Q85" t="n">
+        <v>157.4326666666667</v>
+      </c>
+      <c r="R85" t="n">
+        <v>187.59</v>
+      </c>
+      <c r="S85" t="n">
+        <v>186.1770762978394</v>
+      </c>
+      <c r="T85" t="n">
+        <v>174.7653556915622</v>
+      </c>
+      <c r="U85" t="n">
+        <v>166.9461493075669</v>
+      </c>
+      <c r="V85" t="n">
+        <v>7.819206383995322</v>
+      </c>
+      <c r="W85" t="n">
+        <v>5.298954343509458</v>
+      </c>
+      <c r="X85" t="n">
+        <v>2.520252040485864</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>187.60000000</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>198.36000000</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>185.76000000</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>194.21000000</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>866478.04928000</t>
+        </is>
+      </c>
+      <c r="G86" t="n">
+        <v>1587859199999</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>167703202.42505130</t>
+        </is>
+      </c>
+      <c r="I86" t="n">
+        <v>244755</v>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>438541.85997000</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>84884022.53154650</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>2020-04-25 08:00:00</t>
+        </is>
+      </c>
+      <c r="M86" t="n">
+        <v>194.2099999999998</v>
+      </c>
+      <c r="N86" t="n">
+        <v>190.9</v>
+      </c>
+      <c r="O86" t="n">
+        <v>181.5685714285714</v>
+      </c>
+      <c r="P86" t="n">
+        <v>172.3833333333334</v>
+      </c>
+      <c r="Q86" t="n">
+        <v>159.293</v>
+      </c>
+      <c r="R86" t="n">
+        <v>194.21</v>
+      </c>
+      <c r="S86" t="n">
+        <v>191.5323587659465</v>
+      </c>
+      <c r="T86" t="n">
+        <v>177.7568414687404</v>
+      </c>
+      <c r="U86" t="n">
+        <v>168.9686102962924</v>
+      </c>
+      <c r="V86" t="n">
+        <v>8.788231172447979</v>
+      </c>
+      <c r="W86" t="n">
+        <v>5.996809713337469</v>
+      </c>
+      <c r="X86" t="n">
+        <v>2.79142145911051</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>194.21000000</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>200.00000000</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>192.30000000</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>197.38000000</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>758525.81533000</t>
+        </is>
+      </c>
+      <c r="G87" t="n">
+        <v>1587945599999</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>148433709.77718670</t>
+        </is>
+      </c>
+      <c r="I87" t="n">
+        <v>228826</v>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>383155.46184000</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>74997367.32236560</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>2020-04-26 08:00:00</t>
+        </is>
+      </c>
+      <c r="M87" t="n">
+        <v>197.3799999999998</v>
+      </c>
+      <c r="N87" t="n">
+        <v>195.795</v>
+      </c>
+      <c r="O87" t="n">
+        <v>184.0471428571429</v>
+      </c>
+      <c r="P87" t="n">
+        <v>174.9866666666667</v>
+      </c>
+      <c r="Q87" t="n">
+        <v>161.4946666666667</v>
+      </c>
+      <c r="R87" t="n">
+        <v>197.38</v>
+      </c>
+      <c r="S87" t="n">
+        <v>195.4307862553155</v>
+      </c>
+      <c r="T87" t="n">
+        <v>180.7757906748844</v>
+      </c>
+      <c r="U87" t="n">
+        <v>171.075971499785</v>
+      </c>
+      <c r="V87" t="n">
+        <v>9.699819175099378</v>
+      </c>
+      <c r="W87" t="n">
+        <v>6.737411609120084</v>
+      </c>
+      <c r="X87" t="n">
+        <v>2.962407565979294</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>197.39000000</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>199.05000000</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>189.29000000</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>196.34000000</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>896627.37271000</t>
+        </is>
+      </c>
+      <c r="G88" t="n">
+        <v>1588031999999</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>174775637.92727570</t>
+        </is>
+      </c>
+      <c r="I88" t="n">
+        <v>238341</v>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>426083.00347000</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>83095117.55550340</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>2020-04-27 08:00:00</t>
+        </is>
+      </c>
+      <c r="M88" t="n">
+        <v>196.3399999999998</v>
+      </c>
+      <c r="N88" t="n">
+        <v>196.86</v>
+      </c>
+      <c r="O88" t="n">
+        <v>187.7814285714286</v>
+      </c>
+      <c r="P88" t="n">
+        <v>177.5033333333334</v>
+      </c>
+      <c r="Q88" t="n">
+        <v>163.6733333333334</v>
+      </c>
+      <c r="R88" t="n">
+        <v>196.34</v>
+      </c>
+      <c r="S88" t="n">
+        <v>196.0369287517718</v>
+      </c>
+      <c r="T88" t="n">
+        <v>183.1702855848415</v>
+      </c>
+      <c r="U88" t="n">
+        <v>172.9496975560001</v>
+      </c>
+      <c r="V88" t="n">
+        <v>10.22058802884141</v>
+      </c>
+      <c r="W88" t="n">
+        <v>7.434046895645624</v>
+      </c>
+      <c r="X88" t="n">
+        <v>2.786541133195781</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>196.33000000</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>198.50000000</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>192.36000000</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>196.24000000</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>636829.89397000</t>
+        </is>
+      </c>
+      <c r="G89" t="n">
+        <v>1588118399999</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>124476041.88938340</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
+        <v>183819</v>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>324710.24289000</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>63499045.65033740</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>2020-04-28 08:00:00</t>
+        </is>
+      </c>
+      <c r="M89" t="n">
+        <v>196.2399999999998</v>
+      </c>
+      <c r="N89" t="n">
+        <v>196.29</v>
+      </c>
+      <c r="O89" t="n">
+        <v>191.4242857142857</v>
+      </c>
+      <c r="P89" t="n">
+        <v>180.1666666666667</v>
+      </c>
+      <c r="Q89" t="n">
+        <v>166.0646666666667</v>
+      </c>
+      <c r="R89" t="n">
+        <v>196.24</v>
+      </c>
+      <c r="S89" t="n">
+        <v>196.1723095839239</v>
+      </c>
+      <c r="T89" t="n">
+        <v>185.18101170913</v>
+      </c>
+      <c r="U89" t="n">
+        <v>174.6768823340517</v>
+      </c>
+      <c r="V89" t="n">
+        <v>10.50412937507824</v>
+      </c>
+      <c r="W89" t="n">
+        <v>8.048063393352262</v>
+      </c>
+      <c r="X89" t="n">
+        <v>2.456065981725974</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>196.24000000</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>218.77000000</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>196.22000000</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>215.36000000</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>1620422.72431000</t>
+        </is>
+      </c>
+      <c r="G90" t="n">
+        <v>1588204799999</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>338324593.63729170</t>
+        </is>
+      </c>
+      <c r="I90" t="n">
+        <v>445147</v>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>817195.35504000</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>170664754.30895850</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>2020-04-29 08:00:00</t>
+        </is>
+      </c>
+      <c r="M90" t="n">
+        <v>215.3599999999998</v>
+      </c>
+      <c r="N90" t="n">
+        <v>205.8</v>
+      </c>
+      <c r="O90" t="n">
+        <v>196.09</v>
+      </c>
+      <c r="P90" t="n">
+        <v>183.9606666666668</v>
+      </c>
+      <c r="Q90" t="n">
+        <v>168.8413333333334</v>
+      </c>
+      <c r="R90" t="n">
+        <v>215.36</v>
+      </c>
+      <c r="S90" t="n">
+        <v>208.9641031946413</v>
+      </c>
+      <c r="T90" t="n">
+        <v>189.823934605645</v>
+      </c>
+      <c r="U90" t="n">
+        <v>177.693644225186</v>
+      </c>
+      <c r="V90" t="n">
+        <v>12.13029038045897</v>
+      </c>
+      <c r="W90" t="n">
+        <v>8.86450879270974</v>
+      </c>
+      <c r="X90" t="n">
+        <v>3.265781587749233</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>215.40000000</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>227.30000000</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>202.00000000</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>206.08000000</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>1749691.00151000</t>
+        </is>
+      </c>
+      <c r="G91" t="n">
+        <v>1588291199999</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>374893029.77430840</t>
+        </is>
+      </c>
+      <c r="I91" t="n">
+        <v>557268</v>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>840566.78901000</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>180276410.99706310</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>2020-04-30 08:00:00</t>
+        </is>
+      </c>
+      <c r="M91" t="n">
+        <v>206.0799999999998</v>
+      </c>
+      <c r="N91" t="n">
+        <v>210.72</v>
+      </c>
+      <c r="O91" t="n">
+        <v>199.0285714285714</v>
+      </c>
+      <c r="P91" t="n">
+        <v>187.5173333333334</v>
+      </c>
+      <c r="Q91" t="n">
+        <v>171.2866666666667</v>
+      </c>
+      <c r="R91" t="n">
+        <v>206.08</v>
+      </c>
+      <c r="S91" t="n">
+        <v>207.0413677315471</v>
+      </c>
+      <c r="T91" t="n">
+        <v>192.324868482064</v>
+      </c>
+      <c r="U91" t="n">
+        <v>179.7984029316126</v>
+      </c>
+      <c r="V91" t="n">
+        <v>12.52646555045143</v>
+      </c>
+      <c r="W91" t="n">
+        <v>9.596900145647526</v>
+      </c>
+      <c r="X91" t="n">
+        <v>2.929565404803908</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>206.07000000</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>217.14000000</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>205.91000000</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>212.02000000</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>794913.95828000</t>
+        </is>
+      </c>
+      <c r="G92" t="n">
+        <v>1588377599999</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>168339123.35791390</t>
+        </is>
+      </c>
+      <c r="I92" t="n">
+        <v>291365</v>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>389989.76909000</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>82585993.16044210</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>2020-05-01 08:00:00</t>
+        </is>
+      </c>
+      <c r="M92" t="n">
+        <v>212.0199999999998</v>
+      </c>
+      <c r="N92" t="n">
+        <v>209.05</v>
+      </c>
+      <c r="O92" t="n">
+        <v>202.5185714285714</v>
+      </c>
+      <c r="P92" t="n">
+        <v>190.1660000000001</v>
+      </c>
+      <c r="Q92" t="n">
+        <v>173.831</v>
+      </c>
+      <c r="R92" t="n">
+        <v>212.02</v>
+      </c>
+      <c r="S92" t="n">
+        <v>210.3604559105157</v>
+      </c>
+      <c r="T92" t="n">
+        <v>195.3548894730094</v>
+      </c>
+      <c r="U92" t="n">
+        <v>182.1873588324577</v>
+      </c>
+      <c r="V92" t="n">
+        <v>13.16753064055169</v>
+      </c>
+      <c r="W92" t="n">
+        <v>10.31102624571219</v>
+      </c>
+      <c r="X92" t="n">
+        <v>2.856504394839495</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>212.01000000</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>215.37000000</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>210.36000000</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>213.90000000</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>443494.67248000</t>
+        </is>
+      </c>
+      <c r="G93" t="n">
+        <v>1588463999999</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>94389501.51781640</t>
+        </is>
+      </c>
+      <c r="I93" t="n">
+        <v>185802</v>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>225155.58197000</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>47928012.23135540</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>2020-05-02 08:00:00</t>
+        </is>
+      </c>
+      <c r="M93" t="n">
+        <v>213.8999999999998</v>
+      </c>
+      <c r="N93" t="n">
+        <v>212.96</v>
+      </c>
+      <c r="O93" t="n">
+        <v>205.3314285714286</v>
+      </c>
+      <c r="P93" t="n">
+        <v>193.0466666666667</v>
+      </c>
+      <c r="Q93" t="n">
+        <v>176.2516666666667</v>
+      </c>
+      <c r="R93" t="n">
+        <v>213.9</v>
+      </c>
+      <c r="S93" t="n">
+        <v>212.7201519701719</v>
+      </c>
+      <c r="T93" t="n">
+        <v>198.2079840037075</v>
+      </c>
+      <c r="U93" t="n">
+        <v>184.5384216022044</v>
+      </c>
+      <c r="V93" t="n">
+        <v>13.6695624015031</v>
+      </c>
+      <c r="W93" t="n">
+        <v>10.98273347768594</v>
+      </c>
+      <c r="X93" t="n">
+        <v>2.686828923817158</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>213.89000000</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>219.30000000</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>203.92000000</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>209.86000000</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>748383.91311000</t>
+        </is>
+      </c>
+      <c r="G94" t="n">
+        <v>1588550399999</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>158874887.07834110</t>
+        </is>
+      </c>
+      <c r="I94" t="n">
+        <v>268841</v>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>354161.96792000</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>75207830.89534740</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>2020-05-03 08:00:00</t>
+        </is>
+      </c>
+      <c r="M94" t="n">
+        <v>209.8599999999998</v>
+      </c>
+      <c r="N94" t="n">
+        <v>211.88</v>
+      </c>
+      <c r="O94" t="n">
+        <v>207.1142857142857</v>
+      </c>
+      <c r="P94" t="n">
+        <v>194.5440000000001</v>
+      </c>
+      <c r="Q94" t="n">
+        <v>178.5366666666667</v>
+      </c>
+      <c r="R94" t="n">
+        <v>209.86</v>
+      </c>
+      <c r="S94" t="n">
+        <v>210.8133839900573</v>
+      </c>
+      <c r="T94" t="n">
+        <v>200.0006021701216</v>
+      </c>
+      <c r="U94" t="n">
+        <v>186.4155565436485</v>
+      </c>
+      <c r="V94" t="n">
+        <v>13.58504562647306</v>
+      </c>
+      <c r="W94" t="n">
+        <v>11.50319590794891</v>
+      </c>
+      <c r="X94" t="n">
+        <v>2.081849718524152</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>209.86000000</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>210.65000000</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>194.88000000</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>206.48000000</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>1114249.32658000</t>
+        </is>
+      </c>
+      <c r="G95" t="n">
+        <v>1588636799999</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>225451167.65536830</t>
+        </is>
+      </c>
+      <c r="I95" t="n">
+        <v>349701</v>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>553422.13712000</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>111948053.08533100</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>2020-05-04 08:00:00</t>
+        </is>
+      </c>
+      <c r="M95" t="n">
+        <v>206.4799999999997</v>
+      </c>
+      <c r="N95" t="n">
+        <v>208.17</v>
+      </c>
+      <c r="O95" t="n">
+        <v>208.5628571428571</v>
+      </c>
+      <c r="P95" t="n">
+        <v>196.3073333333334</v>
+      </c>
+      <c r="Q95" t="n">
+        <v>180.616</v>
+      </c>
+      <c r="R95" t="n">
+        <v>206.48</v>
+      </c>
+      <c r="S95" t="n">
+        <v>207.9244613300191</v>
+      </c>
+      <c r="T95" t="n">
+        <v>200.9974327564464</v>
+      </c>
+      <c r="U95" t="n">
+        <v>187.9028845502985</v>
+      </c>
+      <c r="V95" t="n">
+        <v>13.09454820614783</v>
+      </c>
+      <c r="W95" t="n">
+        <v>11.82146636783601</v>
+      </c>
+      <c r="X95" t="n">
+        <v>1.273081838311825</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>206.47000000</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>211.68000000</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>201.00000000</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>205.29000000</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>640644.66268000</t>
+        </is>
+      </c>
+      <c r="G96" t="n">
+        <v>1588723199999</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>131906204.90781300</t>
+        </is>
+      </c>
+      <c r="I96" t="n">
+        <v>246124</v>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>310794.78031000</t>
+        </is>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>64025329.18628990</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>2020-05-05 08:00:00</t>
+        </is>
+      </c>
+      <c r="M96" t="n">
+        <v>205.2899999999998</v>
+      </c>
+      <c r="N96" t="n">
+        <v>205.885</v>
+      </c>
+      <c r="O96" t="n">
+        <v>209.8557142857142</v>
+      </c>
+      <c r="P96" t="n">
+        <v>198.6466666666667</v>
+      </c>
+      <c r="Q96" t="n">
+        <v>182.703</v>
+      </c>
+      <c r="R96" t="n">
+        <v>205.29</v>
+      </c>
+      <c r="S96" t="n">
+        <v>206.168153776673</v>
+      </c>
+      <c r="T96" t="n">
+        <v>201.6578278016165</v>
+      </c>
+      <c r="U96" t="n">
+        <v>189.191679877455</v>
+      </c>
+      <c r="V96" t="n">
+        <v>12.46614792416148</v>
+      </c>
+      <c r="W96" t="n">
+        <v>11.95040267918126</v>
+      </c>
+      <c r="X96" t="n">
+        <v>0.5157452449802182</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>205.30000000</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>210.77000000</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>197.71000000</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>198.97000000</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>862700.67849000</t>
+        </is>
+      </c>
+      <c r="G97" t="n">
+        <v>1588809599999</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>178157452.60084120</t>
+        </is>
+      </c>
+      <c r="I97" t="n">
+        <v>271299</v>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>411115.12204000</t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>84998478.60793140</t>
+        </is>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>2020-05-06 08:00:00</t>
+        </is>
+      </c>
+      <c r="M97" t="n">
+        <v>198.9699999999998</v>
+      </c>
+      <c r="N97" t="n">
+        <v>202.13</v>
+      </c>
+      <c r="O97" t="n">
+        <v>207.5142857142857</v>
+      </c>
+      <c r="P97" t="n">
+        <v>200.5286666666667</v>
+      </c>
+      <c r="Q97" t="n">
+        <v>183.6246666666667</v>
+      </c>
+      <c r="R97" t="n">
+        <v>198.97</v>
+      </c>
+      <c r="S97" t="n">
+        <v>201.3693845922243</v>
+      </c>
+      <c r="T97" t="n">
+        <v>201.2443157873013</v>
+      </c>
+      <c r="U97" t="n">
+        <v>189.9164481348184</v>
+      </c>
+      <c r="V97" t="n">
+        <v>11.32786765248295</v>
+      </c>
+      <c r="W97" t="n">
+        <v>11.82589567377968</v>
+      </c>
+      <c r="X97" t="n">
+        <v>-0.4980280212967259</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>198.92000000</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>215.10000000</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>196.43000000</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>212.00000000</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>1305778.73764000</t>
+        </is>
+      </c>
+      <c r="G98" t="n">
+        <v>1588895999999</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>271197927.66502780</t>
+        </is>
+      </c>
+      <c r="I98" t="n">
+        <v>380313</v>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>660789.67892000</t>
+        </is>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>137272634.80833200</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>2020-05-07 08:00:00</t>
+        </is>
+      </c>
+      <c r="M98" t="n">
+        <v>211.9999999999998</v>
+      </c>
+      <c r="N98" t="n">
+        <v>205.485</v>
+      </c>
+      <c r="O98" t="n">
+        <v>208.36</v>
+      </c>
+      <c r="P98" t="n">
+        <v>202.4820000000001</v>
+      </c>
+      <c r="Q98" t="n">
+        <v>185.2036666666667</v>
+      </c>
+      <c r="R98" t="n">
+        <v>212</v>
+      </c>
+      <c r="S98" t="n">
+        <v>208.4564615307414</v>
+      </c>
+      <c r="T98" t="n">
+        <v>202.8990365872222</v>
+      </c>
+      <c r="U98" t="n">
+        <v>191.5532040937246</v>
+      </c>
+      <c r="V98" t="n">
+        <v>11.34583249349754</v>
+      </c>
+      <c r="W98" t="n">
+        <v>11.72988303768505</v>
+      </c>
+      <c r="X98" t="n">
+        <v>-0.3840505441875113</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>212.01000000</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>216.61000000</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>206.90000000</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>211.31000000</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>917908.19440000</t>
+        </is>
+      </c>
+      <c r="G99" t="n">
+        <v>1588982399999</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>194579529.42776330</t>
+        </is>
+      </c>
+      <c r="I99" t="n">
+        <v>262122</v>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>445600.39696000</t>
+        </is>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>94465691.13477140</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>2020-05-08 08:00:00</t>
+        </is>
+      </c>
+      <c r="M99" t="n">
+        <v>211.3099999999998</v>
+      </c>
+      <c r="N99" t="n">
+        <v>211.655</v>
+      </c>
+      <c r="O99" t="n">
+        <v>208.2585714285714</v>
+      </c>
+      <c r="P99" t="n">
+        <v>204.2020000000001</v>
+      </c>
+      <c r="Q99" t="n">
+        <v>186.477</v>
+      </c>
+      <c r="R99" t="n">
+        <v>211.31</v>
+      </c>
+      <c r="S99" t="n">
+        <v>210.3588205102471</v>
+      </c>
+      <c r="T99" t="n">
+        <v>204.1930310588727</v>
+      </c>
+      <c r="U99" t="n">
+        <v>193.0174468562973</v>
+      </c>
+      <c r="V99" t="n">
+        <v>11.17558420257544</v>
+      </c>
+      <c r="W99" t="n">
+        <v>11.61902327062784</v>
+      </c>
+      <c r="X99" t="n">
+        <v>-0.4434390680524061</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>211.32000000</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>214.60000000</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>208.40000000</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>210.07000000</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>587871.98073000</t>
+        </is>
+      </c>
+      <c r="G100" t="n">
+        <v>1589068799999</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>124626471.42703530</t>
+        </is>
+      </c>
+      <c r="I100" t="n">
+        <v>194059</v>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>292187.26718000</t>
+        </is>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>61966403.94492970</t>
+        </is>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>2020-05-09 08:00:00</t>
+        </is>
+      </c>
+      <c r="M100" t="n">
+        <v>210.0699999999998</v>
+      </c>
+      <c r="N100" t="n">
+        <v>210.6899999999999</v>
+      </c>
+      <c r="O100" t="n">
+        <v>207.7114285714285</v>
+      </c>
+      <c r="P100" t="n">
+        <v>205.7006666666668</v>
+      </c>
+      <c r="Q100" t="n">
+        <v>187.8286666666667</v>
+      </c>
+      <c r="R100" t="n">
+        <v>210.07</v>
+      </c>
+      <c r="S100" t="n">
+        <v>210.1662735034157</v>
+      </c>
+      <c r="T100" t="n">
+        <v>205.0971801861299</v>
+      </c>
+      <c r="U100" t="n">
+        <v>194.2812194057821</v>
+      </c>
+      <c r="V100" t="n">
+        <v>10.81596078034775</v>
+      </c>
+      <c r="W100" t="n">
+        <v>11.45841077253093</v>
+      </c>
+      <c r="X100" t="n">
+        <v>-0.6424499921831757</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>210.09000000</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>210.18000000</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>179.59000000</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>187.54000000</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>1473226.05475000</t>
+        </is>
+      </c>
+      <c r="G101" t="n">
+        <v>1589155199999</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>278394290.75973460</t>
+        </is>
+      </c>
+      <c r="I101" t="n">
+        <v>426358</v>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>694788.42914000</t>
+        </is>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>131143494.26749300</t>
+        </is>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>2020-05-10 08:00:00</t>
+        </is>
+      </c>
+      <c r="M101" t="n">
+        <v>187.5399999999998</v>
+      </c>
+      <c r="N101" t="n">
+        <v>198.8049999999999</v>
+      </c>
+      <c r="O101" t="n">
+        <v>204.5228571428571</v>
+      </c>
+      <c r="P101" t="n">
+        <v>205.2560000000001</v>
+      </c>
+      <c r="Q101" t="n">
+        <v>188.8196666666666</v>
+      </c>
+      <c r="R101" t="n">
+        <v>187.54</v>
+      </c>
+      <c r="S101" t="n">
+        <v>195.0820911678053</v>
+      </c>
+      <c r="T101" t="n">
+        <v>202.3960753919774</v>
+      </c>
+      <c r="U101" t="n">
+        <v>193.7816427152093</v>
+      </c>
+      <c r="V101" t="n">
+        <v>8.614432676768047</v>
+      </c>
+      <c r="W101" t="n">
+        <v>10.88961515326248</v>
+      </c>
+      <c r="X101" t="n">
+        <v>-2.275182476494438</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>187.62000000</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>193.50000000</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>176.00000000</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>185.73000000</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>1093299.81927000</t>
+        </is>
+      </c>
+      <c r="G102" t="n">
+        <v>1589241599999</v>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>203391530.20617390</t>
+        </is>
+      </c>
+      <c r="I102" t="n">
+        <v>303669</v>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>529158.74668000</t>
+        </is>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>98465728.22507510</t>
+        </is>
+      </c>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>2020-05-11 08:00:00</t>
+        </is>
+      </c>
+      <c r="M102" t="n">
+        <v>185.7299999999998</v>
+      </c>
+      <c r="N102" t="n">
+        <v>186.6349999999999</v>
+      </c>
+      <c r="O102" t="n">
+        <v>201.5585714285714</v>
+      </c>
+      <c r="P102" t="n">
+        <v>204.4793333333334</v>
+      </c>
+      <c r="Q102" t="n">
+        <v>189.733</v>
+      </c>
+      <c r="R102" t="n">
+        <v>185.73</v>
+      </c>
+      <c r="S102" t="n">
+        <v>188.8473637226017</v>
+      </c>
+      <c r="T102" t="n">
+        <v>199.832063672624</v>
+      </c>
+      <c r="U102" t="n">
+        <v>193.1849735856791</v>
+      </c>
+      <c r="V102" t="n">
+        <v>6.647090086944928</v>
+      </c>
+      <c r="W102" t="n">
+        <v>10.0411101398607</v>
+      </c>
+      <c r="X102" t="n">
+        <v>-3.394020052915771</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>185.80000000</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>192.24000000</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>185.48000000</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>189.76000000</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>669755.79567000</t>
+        </is>
+      </c>
+      <c r="G103" t="n">
+        <v>1589327999999</v>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>126810812.16817080</t>
+        </is>
+      </c>
+      <c r="I103" t="n">
+        <v>193978</v>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>336075.30552000</t>
+        </is>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>63647040.81413890</t>
+        </is>
+      </c>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>2020-05-12 08:00:00</t>
+        </is>
+      </c>
+      <c r="M103" t="n">
+        <v>189.7599999999998</v>
+      </c>
+      <c r="N103" t="n">
+        <v>187.7449999999999</v>
+      </c>
+      <c r="O103" t="n">
+        <v>199.34</v>
+      </c>
+      <c r="P103" t="n">
+        <v>204.0406666666668</v>
+      </c>
+      <c r="Q103" t="n">
+        <v>190.772</v>
+      </c>
+      <c r="R103" t="n">
+        <v>189.76</v>
+      </c>
+      <c r="S103" t="n">
+        <v>189.4557879075339</v>
+      </c>
+      <c r="T103" t="n">
+        <v>198.2825153536325</v>
+      </c>
+      <c r="U103" t="n">
+        <v>192.9311729218747</v>
+      </c>
+      <c r="V103" t="n">
+        <v>5.351342431757757</v>
+      </c>
+      <c r="W103" t="n">
+        <v>9.103156598117829</v>
+      </c>
+      <c r="X103" t="n">
+        <v>-3.751814166360072</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>189.77000000</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>201.00000000</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>188.35000000</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>199.58000000</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>806143.00704000</t>
+        </is>
+      </c>
+      <c r="G104" t="n">
+        <v>1589414399999</v>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>156637596.36492460</t>
+        </is>
+      </c>
+      <c r="I104" t="n">
+        <v>212710</v>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>410843.35618000</t>
+        </is>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>79791107.72434880</t>
+        </is>
+      </c>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t>2020-05-13 08:00:00</t>
+        </is>
+      </c>
+      <c r="M104" t="n">
+        <v>199.5799999999998</v>
+      </c>
+      <c r="N104" t="n">
+        <v>194.6699999999999</v>
+      </c>
+      <c r="O104" t="n">
+        <v>199.4271428571428</v>
+      </c>
+      <c r="P104" t="n">
+        <v>204.2633333333334</v>
+      </c>
+      <c r="Q104" t="n">
+        <v>192.215</v>
+      </c>
+      <c r="R104" t="n">
+        <v>199.58</v>
+      </c>
+      <c r="S104" t="n">
+        <v>196.2052626358446</v>
+      </c>
+      <c r="T104" t="n">
+        <v>198.4821283828721</v>
+      </c>
+      <c r="U104" t="n">
+        <v>193.4238564270467</v>
+      </c>
+      <c r="V104" t="n">
+        <v>5.058271955825461</v>
+      </c>
+      <c r="W104" t="n">
+        <v>8.294179669574982</v>
+      </c>
+      <c r="X104" t="n">
+        <v>-3.235907713749521</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>199.61000000</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>206.02000000</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>195.67000000</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>203.29000000</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>1114700.24937000</t>
+        </is>
+      </c>
+      <c r="G105" t="n">
+        <v>1589500799999</v>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>224233786.12670990</t>
+        </is>
+      </c>
+      <c r="I105" t="n">
+        <v>285245</v>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>557166.15035000</t>
+        </is>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>112099049.73738440</t>
+        </is>
+      </c>
+      <c r="L105" t="inlineStr">
+        <is>
+          <t>2020-05-14 08:00:00</t>
+        </is>
+      </c>
+      <c r="M105" t="n">
+        <v>203.2899999999998</v>
+      </c>
+      <c r="N105" t="n">
+        <v>201.4349999999999</v>
+      </c>
+      <c r="O105" t="n">
+        <v>198.1828571428571</v>
+      </c>
+      <c r="P105" t="n">
+        <v>203.4586666666668</v>
+      </c>
+      <c r="Q105" t="n">
+        <v>193.7096666666666</v>
+      </c>
+      <c r="R105" t="n">
+        <v>203.29</v>
+      </c>
+      <c r="S105" t="n">
+        <v>200.9284208786149</v>
+      </c>
+      <c r="T105" t="n">
+        <v>199.2218009604285</v>
+      </c>
+      <c r="U105" t="n">
+        <v>194.1549261570753</v>
+      </c>
+      <c r="V105" t="n">
+        <v>5.066874803353187</v>
+      </c>
+      <c r="W105" t="n">
+        <v>7.648718696276768</v>
+      </c>
+      <c r="X105" t="n">
+        <v>-2.581843892923581</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>203.29000000</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>204.08000000</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>191.66000000</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>194.86000000</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>904749.63570000</t>
+        </is>
+      </c>
+      <c r="G106" t="n">
+        <v>1589587199999</v>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>179634085.62276920</t>
+        </is>
+      </c>
+      <c r="I106" t="n">
+        <v>230721</v>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>437768.77270000</t>
+        </is>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>86944450.76006710</t>
+        </is>
+      </c>
+      <c r="L106" t="inlineStr">
+        <is>
+          <t>2020-05-15 08:00:00</t>
+        </is>
+      </c>
+      <c r="M106" t="n">
+        <v>194.8599999999998</v>
+      </c>
+      <c r="N106" t="n">
+        <v>199.0749999999999</v>
+      </c>
+      <c r="O106" t="n">
+        <v>195.8328571428571</v>
+      </c>
+      <c r="P106" t="n">
+        <v>202.7106666666668</v>
+      </c>
+      <c r="Q106" t="n">
+        <v>195.114</v>
+      </c>
+      <c r="R106" t="n">
+        <v>194.86</v>
+      </c>
+      <c r="S106" t="n">
+        <v>196.8828069595383</v>
+      </c>
+      <c r="T106" t="n">
+        <v>198.5507546426458</v>
+      </c>
+      <c r="U106" t="n">
+        <v>194.207170012848</v>
+      </c>
+      <c r="V106" t="n">
+        <v>4.343584629797789</v>
+      </c>
+      <c r="W106" t="n">
+        <v>6.987691882936851</v>
+      </c>
+      <c r="X106" t="n">
+        <v>-2.644107253139062</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>194.87000000</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>203.50000000</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>193.21000000</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>200.45000000</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>669900.03754000</t>
+        </is>
+      </c>
+      <c r="G107" t="n">
+        <v>1589673599999</v>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>134060788.49418390</t>
+        </is>
+      </c>
+      <c r="I107" t="n">
+        <v>174447</v>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>343539.34568000</t>
+        </is>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>68751336.84186420</t>
+        </is>
+      </c>
+      <c r="L107" t="inlineStr">
+        <is>
+          <t>2020-05-16 08:00:00</t>
+        </is>
+      </c>
+      <c r="M107" t="n">
+        <v>200.4499999999997</v>
+      </c>
+      <c r="N107" t="n">
+        <v>197.6549999999999</v>
+      </c>
+      <c r="O107" t="n">
+        <v>194.4585714285714</v>
+      </c>
+      <c r="P107" t="n">
+        <v>201.9393333333334</v>
+      </c>
+      <c r="Q107" t="n">
+        <v>196.0526666666666</v>
+      </c>
+      <c r="R107" t="n">
+        <v>200.45</v>
+      </c>
+      <c r="S107" t="n">
+        <v>199.2609356531794</v>
+      </c>
+      <c r="T107" t="n">
+        <v>198.8429462420456</v>
+      </c>
+      <c r="U107" t="n">
+        <v>194.6697343754064</v>
+      </c>
+      <c r="V107" t="n">
+        <v>4.173211866639235</v>
+      </c>
+      <c r="W107" t="n">
+        <v>6.424795879647268</v>
+      </c>
+      <c r="X107" t="n">
+        <v>-2.251584013008032</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>200.44000000</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>209.85000000</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>199.68000000</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>207.00000000</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>708711.89315000</t>
+        </is>
+      </c>
+      <c r="G108" t="n">
+        <v>1589759999999</v>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>145341278.68135490</t>
+        </is>
+      </c>
+      <c r="I108" t="n">
+        <v>180088</v>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>369150.31059000</t>
+        </is>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>75677871.47041410</t>
+        </is>
+      </c>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>2020-05-17 08:00:00</t>
+        </is>
+      </c>
+      <c r="M108" t="n">
+        <v>206.9999999999997</v>
+      </c>
+      <c r="N108" t="n">
+        <v>203.7249999999999</v>
+      </c>
+      <c r="O108" t="n">
+        <v>197.2385714285714</v>
+      </c>
+      <c r="P108" t="n">
+        <v>201.4793333333334</v>
+      </c>
+      <c r="Q108" t="n">
+        <v>197.263</v>
+      </c>
+      <c r="R108" t="n">
+        <v>207</v>
+      </c>
+      <c r="S108" t="n">
+        <v>204.4203118843932</v>
+      </c>
+      <c r="T108" t="n">
+        <v>200.0978776110852</v>
+      </c>
+      <c r="U108" t="n">
+        <v>195.5833297173458</v>
+      </c>
+      <c r="V108" t="n">
+        <v>4.514547893739433</v>
+      </c>
+      <c r="W108" t="n">
+        <v>6.042746282449381</v>
+      </c>
+      <c r="X108" t="n">
+        <v>-1.528198388709948</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>207.02000000</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>217.07000000</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>207.00000000</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>214.91000000</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>1064139.24850000</t>
+        </is>
+      </c>
+      <c r="G109" t="n">
+        <v>1589846399999</v>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>226789027.15008040</t>
+        </is>
+      </c>
+      <c r="I109" t="n">
+        <v>249528</v>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>538438.67639000</t>
+        </is>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>114784967.15147500</t>
+        </is>
+      </c>
+      <c r="L109" t="inlineStr">
+        <is>
+          <t>2020-05-18 08:00:00</t>
+        </is>
+      </c>
+      <c r="M109" t="n">
+        <v>214.9099999999997</v>
+      </c>
+      <c r="N109" t="n">
+        <v>210.9549999999998</v>
+      </c>
+      <c r="O109" t="n">
+        <v>201.4071428571429</v>
+      </c>
+      <c r="P109" t="n">
+        <v>201.8160000000001</v>
+      </c>
+      <c r="Q109" t="n">
+        <v>198.18</v>
+      </c>
+      <c r="R109" t="n">
+        <v>214.91</v>
+      </c>
+      <c r="S109" t="n">
+        <v>211.4134372947977</v>
+      </c>
+      <c r="T109" t="n">
+        <v>202.376665704202</v>
+      </c>
+      <c r="U109" t="n">
+        <v>197.015286616978</v>
+      </c>
+      <c r="V109" t="n">
+        <v>5.361379087223924</v>
+      </c>
+      <c r="W109" t="n">
+        <v>5.906472843399632</v>
+      </c>
+      <c r="X109" t="n">
+        <v>-0.5450937561757083</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>214.92000000</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>215.95000000</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>209.45000000</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>214.58000000</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>643702.98849000</t>
+        </is>
+      </c>
+      <c r="G110" t="n">
+        <v>1589932799999</v>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>136846948.55680560</t>
+        </is>
+      </c>
+      <c r="I110" t="n">
+        <v>186027</v>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>319009.59630000</t>
+        </is>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>67835348.16258670</t>
+        </is>
+      </c>
+      <c r="L110" t="inlineStr">
+        <is>
+          <t>2020-05-19 08:00:00</t>
+        </is>
+      </c>
+      <c r="M110" t="n">
+        <v>214.5799999999998</v>
+      </c>
+      <c r="N110" t="n">
+        <v>214.7449999999998</v>
+      </c>
+      <c r="O110" t="n">
+        <v>204.9528571428571</v>
+      </c>
+      <c r="P110" t="n">
+        <v>202.3560000000001</v>
+      </c>
+      <c r="Q110" t="n">
+        <v>199.3316666666666</v>
+      </c>
+      <c r="R110" t="n">
+        <v>214.58</v>
+      </c>
+      <c r="S110" t="n">
+        <v>213.5244790982659</v>
+      </c>
+      <c r="T110" t="n">
+        <v>204.2541017729123</v>
+      </c>
+      <c r="U110" t="n">
+        <v>198.3166724460986</v>
+      </c>
+      <c r="V110" t="n">
+        <v>5.937429326813657</v>
+      </c>
+      <c r="W110" t="n">
+        <v>5.912664140082607</v>
+      </c>
+      <c r="X110" t="n">
+        <v>0.02476518673104966</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>214.60000000</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>215.75000000</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>204.27000000</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>209.98000000</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>679532.61037000</t>
+        </is>
+      </c>
+      <c r="G111" t="n">
+        <v>1590019199999</v>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>143704806.17524080</t>
+        </is>
+      </c>
+      <c r="I111" t="n">
+        <v>195172</v>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>330890.78825000</t>
+        </is>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>70009379.65600590</t>
+        </is>
+      </c>
+      <c r="L111" t="inlineStr">
+        <is>
+          <t>2020-05-20 08:00:00</t>
+        </is>
+      </c>
+      <c r="M111" t="n">
+        <v>209.9799999999998</v>
+      </c>
+      <c r="N111" t="n">
+        <v>212.2799999999999</v>
+      </c>
+      <c r="O111" t="n">
+        <v>206.4385714285715</v>
+      </c>
+      <c r="P111" t="n">
+        <v>202.6686666666668</v>
+      </c>
+      <c r="Q111" t="n">
+        <v>200.6576666666666</v>
+      </c>
+      <c r="R111" t="n">
+        <v>209.98</v>
+      </c>
+      <c r="S111" t="n">
+        <v>211.1614930327553</v>
+      </c>
+      <c r="T111" t="n">
+        <v>205.1350092016763</v>
+      </c>
+      <c r="U111" t="n">
+        <v>199.1808045915599</v>
+      </c>
+      <c r="V111" t="n">
+        <v>5.954204610116392</v>
+      </c>
+      <c r="W111" t="n">
+        <v>5.920972234089546</v>
+      </c>
+      <c r="X111" t="n">
+        <v>0.03323237602684603</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>209.99000000</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>211.64000000</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>191.71000000</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>198.74000000</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>1003923.43420000</t>
+        </is>
+      </c>
+      <c r="G112" t="n">
+        <v>1590105599999</v>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>203445710.96284490</t>
+        </is>
+      </c>
+      <c r="I112" t="n">
+        <v>258415</v>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>479372.00860000</t>
+        </is>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>97136468.80798330</t>
+        </is>
+      </c>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>2020-05-21 08:00:00</t>
+        </is>
+      </c>
+      <c r="M112" t="n">
+        <v>198.7399999999998</v>
+      </c>
+      <c r="N112" t="n">
+        <v>204.3599999999998</v>
+      </c>
+      <c r="O112" t="n">
+        <v>205.7885714285715</v>
+      </c>
+      <c r="P112" t="n">
+        <v>202.6533333333334</v>
+      </c>
+      <c r="Q112" t="n">
+        <v>201.591</v>
+      </c>
+      <c r="R112" t="n">
+        <v>198.74</v>
+      </c>
+      <c r="S112" t="n">
+        <v>202.8804976775851</v>
+      </c>
+      <c r="T112" t="n">
+        <v>204.1511616234819</v>
+      </c>
+      <c r="U112" t="n">
+        <v>199.1481460322214</v>
+      </c>
+      <c r="V112" t="n">
+        <v>5.003015591260549</v>
+      </c>
+      <c r="W112" t="n">
+        <v>5.737380905520533</v>
+      </c>
+      <c r="X112" t="n">
+        <v>-0.7343653142599837</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>198.72000000</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>209.19000000</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>196.24000000</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>207.36000000</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>787672.36081000</t>
+        </is>
+      </c>
+      <c r="G113" t="n">
+        <v>1590191999999</v>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>159972608.53416610</t>
+        </is>
+      </c>
+      <c r="I113" t="n">
+        <v>217659</v>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>399523.04157000</t>
+        </is>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>81120762.57728450</t>
+        </is>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>2020-05-22 08:00:00</t>
+        </is>
+      </c>
+      <c r="M113" t="n">
+        <v>207.3599999999998</v>
+      </c>
+      <c r="N113" t="n">
+        <v>203.0499999999998</v>
+      </c>
+      <c r="O113" t="n">
+        <v>207.5742857142857</v>
+      </c>
+      <c r="P113" t="n">
+        <v>202.3440000000001</v>
+      </c>
+      <c r="Q113" t="n">
+        <v>202.413</v>
+      </c>
+      <c r="R113" t="n">
+        <v>207.36</v>
+      </c>
+      <c r="S113" t="n">
+        <v>205.866832559195</v>
+      </c>
+      <c r="T113" t="n">
+        <v>204.6448290697194</v>
+      </c>
+      <c r="U113" t="n">
+        <v>199.7565413423933</v>
+      </c>
+      <c r="V113" t="n">
+        <v>4.888287727326087</v>
+      </c>
+      <c r="W113" t="n">
+        <v>5.567562269879267</v>
+      </c>
+      <c r="X113" t="n">
+        <v>-0.6792745425531796</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>207.36000000</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>211.20000000</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>204.55000000</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>206.60000000</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>478559.92006000</t>
+        </is>
+      </c>
+      <c r="G114" t="n">
+        <v>1590278399999</v>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>99461068.10466470</t>
+        </is>
+      </c>
+      <c r="I114" t="n">
+        <v>150729</v>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>237372.30187000</t>
+        </is>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>49341950.41533750</t>
+        </is>
+      </c>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>2020-05-23 08:00:00</t>
+        </is>
+      </c>
+      <c r="M114" t="n">
+        <v>206.5999999999998</v>
+      </c>
+      <c r="N114" t="n">
+        <v>206.9799999999998</v>
+      </c>
+      <c r="O114" t="n">
+        <v>208.4528571428571</v>
+      </c>
+      <c r="P114" t="n">
+        <v>202.0300000000001</v>
+      </c>
+      <c r="Q114" t="n">
+        <v>203.116</v>
+      </c>
+      <c r="R114" t="n">
+        <v>206.6</v>
+      </c>
+      <c r="S114" t="n">
+        <v>206.355610853065</v>
+      </c>
+      <c r="T114" t="n">
+        <v>204.9456245993605</v>
+      </c>
+      <c r="U114" t="n">
+        <v>200.2635489540469</v>
+      </c>
+      <c r="V114" t="n">
+        <v>4.682075645313631</v>
+      </c>
+      <c r="W114" t="n">
+        <v>5.390464944964156</v>
+      </c>
+      <c r="X114" t="n">
+        <v>-0.7083892996505252</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>206.60000000</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>210.55000000</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>199.50000000</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>199.90000000</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>673535.05784000</t>
+        </is>
+      </c>
+      <c r="G115" t="n">
+        <v>1590364799999</v>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>138917619.23362070</t>
+        </is>
+      </c>
+      <c r="I115" t="n">
+        <v>204534</v>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>324023.32350000</t>
+        </is>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>66890503.37754660</t>
+        </is>
+      </c>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>2020-05-24 08:00:00</t>
+        </is>
+      </c>
+      <c r="M115" t="n">
+        <v>199.8999999999998</v>
+      </c>
+      <c r="N115" t="n">
+        <v>203.2499999999998</v>
+      </c>
+      <c r="O115" t="n">
+        <v>207.4385714285714</v>
+      </c>
+      <c r="P115" t="n">
+        <v>201.3520000000001</v>
+      </c>
+      <c r="Q115" t="n">
+        <v>203.5263333333333</v>
+      </c>
+      <c r="R115" t="n">
+        <v>199.9</v>
+      </c>
+      <c r="S115" t="n">
+        <v>202.051870284355</v>
+      </c>
+      <c r="T115" t="n">
+        <v>204.1693746568361</v>
+      </c>
+      <c r="U115" t="n">
+        <v>200.2366152333144</v>
+      </c>
+      <c r="V115" t="n">
+        <v>3.932759423521674</v>
+      </c>
+      <c r="W115" t="n">
+        <v>5.098923840673049</v>
+      </c>
+      <c r="X115" t="n">
+        <v>-1.166164417151375</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>199.90000000</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>205.67000000</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>198.01000000</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>204.15000000</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>469931.62492000</t>
+        </is>
+      </c>
+      <c r="G116" t="n">
+        <v>1590451199999</v>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>95411610.79763470</t>
+        </is>
+      </c>
+      <c r="I116" t="n">
+        <v>171792</v>
+      </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>243595.47559000</t>
+        </is>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>49464529.60504250</t>
+        </is>
+      </c>
+      <c r="L116" t="inlineStr">
+        <is>
+          <t>2020-05-25 08:00:00</t>
+        </is>
+      </c>
+      <c r="M116" t="n">
+        <v>204.1499999999998</v>
+      </c>
+      <c r="N116" t="n">
+        <v>202.0249999999998</v>
+      </c>
+      <c r="O116" t="n">
+        <v>205.9014285714286</v>
+      </c>
+      <c r="P116" t="n">
+        <v>202.4593333333334</v>
+      </c>
+      <c r="Q116" t="n">
+        <v>203.8576666666666</v>
+      </c>
+      <c r="R116" t="n">
+        <v>204.15</v>
+      </c>
+      <c r="S116" t="n">
+        <v>203.4506234281183</v>
+      </c>
+      <c r="T116" t="n">
+        <v>204.1663939403863</v>
+      </c>
+      <c r="U116" t="n">
+        <v>200.5265371343085</v>
+      </c>
+      <c r="V116" t="n">
+        <v>3.639856806077802</v>
+      </c>
+      <c r="W116" t="n">
+        <v>4.807110433751907</v>
+      </c>
+      <c r="X116" t="n">
+        <v>-1.167253627674105</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>204.22000000</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>205.00000000</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>196.90000000</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>200.89000000</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>477176.73530000</t>
+        </is>
+      </c>
+      <c r="G117" t="n">
+        <v>1590537599999</v>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>96116808.85809130</t>
+        </is>
+      </c>
+      <c r="I117" t="n">
+        <v>167702</v>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>233833.77929000</t>
+        </is>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>47132325.29336320</t>
+        </is>
+      </c>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t>2020-05-26 08:00:00</t>
+        </is>
+      </c>
+      <c r="M117" t="n">
+        <v>200.8899999999997</v>
+      </c>
+      <c r="N117" t="n">
+        <v>202.5199999999998</v>
+      </c>
+      <c r="O117" t="n">
+        <v>203.9457142857143</v>
+      </c>
+      <c r="P117" t="n">
+        <v>203.4700000000001</v>
+      </c>
+      <c r="Q117" t="n">
+        <v>203.9746666666666</v>
+      </c>
+      <c r="R117" t="n">
+        <v>200.89</v>
+      </c>
+      <c r="S117" t="n">
+        <v>201.7435411427061</v>
+      </c>
+      <c r="T117" t="n">
+        <v>203.6623333322383</v>
+      </c>
+      <c r="U117" t="n">
+        <v>200.5534638825059</v>
+      </c>
+      <c r="V117" t="n">
+        <v>3.108869449732452</v>
+      </c>
+      <c r="W117" t="n">
+        <v>4.467462236946069</v>
+      </c>
+      <c r="X117" t="n">
+        <v>-1.358592787213617</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>200.92000000</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>208.44000000</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>200.76000000</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>208.29000000</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>494816.72727000</t>
+        </is>
+      </c>
+      <c r="G118" t="n">
+        <v>1590623999999</v>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>101445351.02566320</t>
+        </is>
+      </c>
+      <c r="I118" t="n">
+        <v>167619</v>
+      </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>252824.22653000</t>
+        </is>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>51832733.59846020</t>
+        </is>
+      </c>
+      <c r="L118" t="inlineStr">
+        <is>
+          <t>2020-05-27 08:00:00</t>
+        </is>
+      </c>
+      <c r="M118" t="n">
+        <v>208.2899999999997</v>
+      </c>
+      <c r="N118" t="n">
+        <v>204.5899999999998</v>
+      </c>
+      <c r="O118" t="n">
+        <v>203.7042857142857</v>
+      </c>
+      <c r="P118" t="n">
+        <v>204.7053333333334</v>
+      </c>
+      <c r="Q118" t="n">
+        <v>204.373</v>
+      </c>
+      <c r="R118" t="n">
+        <v>208.29</v>
+      </c>
+      <c r="S118" t="n">
+        <v>206.1078470475687</v>
+      </c>
+      <c r="T118" t="n">
+        <v>204.3742820526677</v>
+      </c>
+      <c r="U118" t="n">
+        <v>201.1266110504481</v>
+      </c>
+      <c r="V118" t="n">
+        <v>3.24767100221959</v>
+      </c>
+      <c r="W118" t="n">
+        <v>4.223503989999654</v>
+      </c>
+      <c r="X118" t="n">
+        <v>-0.9758329877800636</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>208.29000000</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>220.50000000</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>204.67000000</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>220.21000000</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>643945.97769000</t>
+        </is>
+      </c>
+      <c r="G119" t="n">
+        <v>1590710399999</v>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>136361627.34641550</t>
+        </is>
+      </c>
+      <c r="I119" t="n">
+        <v>219160</v>
+      </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>352366.88360000</t>
+        </is>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>74663823.75714590</t>
+        </is>
+      </c>
+      <c r="L119" t="inlineStr">
+        <is>
+          <t>2020-05-28 08:00:00</t>
+        </is>
+      </c>
+      <c r="M119" t="n">
+        <v>220.2099999999998</v>
+      </c>
+      <c r="N119" t="n">
+        <v>214.2499999999998</v>
+      </c>
+      <c r="O119" t="n">
+        <v>206.7714285714285</v>
+      </c>
+      <c r="P119" t="n">
+        <v>206.0806666666668</v>
+      </c>
+      <c r="Q119" t="n">
+        <v>205.172</v>
+      </c>
+      <c r="R119" t="n">
+        <v>220.21</v>
+      </c>
+      <c r="S119" t="n">
+        <v>215.5092823491896</v>
+      </c>
+      <c r="T119" t="n">
+        <v>206.8105463589522</v>
+      </c>
+      <c r="U119" t="n">
+        <v>202.5403562474271</v>
+      </c>
+      <c r="V119" t="n">
+        <v>4.270190111525125</v>
+      </c>
+      <c r="W119" t="n">
+        <v>4.232841214304782</v>
+      </c>
+      <c r="X119" t="n">
+        <v>0.03734889722034218</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>220.24000000</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>224.79000000</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>217.57000000</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>220.67000000</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>603058.07590000</t>
+        </is>
+      </c>
+      <c r="G120" t="n">
+        <v>1590796799999</v>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>133220045.49547060</t>
+        </is>
+      </c>
+      <c r="I120" t="n">
+        <v>217959</v>
+      </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>301826.51829000</t>
+        </is>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>66680504.40036720</t>
+        </is>
+      </c>
+      <c r="L120" t="inlineStr">
+        <is>
+          <t>2020-05-29 08:00:00</t>
+        </is>
+      </c>
+      <c r="M120" t="n">
+        <v>220.6699999999998</v>
+      </c>
+      <c r="N120" t="n">
+        <v>220.4399999999998</v>
+      </c>
+      <c r="O120" t="n">
+        <v>208.6728571428571</v>
+      </c>
+      <c r="P120" t="n">
+        <v>207.2393333333335</v>
+      </c>
+      <c r="Q120" t="n">
+        <v>205.349</v>
+      </c>
+      <c r="R120" t="n">
+        <v>220.67</v>
+      </c>
+      <c r="S120" t="n">
+        <v>218.9497607830632</v>
+      </c>
+      <c r="T120" t="n">
+        <v>208.9427700009944</v>
+      </c>
+      <c r="U120" t="n">
+        <v>203.8834342949474</v>
+      </c>
+      <c r="V120" t="n">
+        <v>5.059335706047079</v>
+      </c>
+      <c r="W120" t="n">
+        <v>4.398140112653727</v>
+      </c>
+      <c r="X120" t="n">
+        <v>0.6611955933933524</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>220.63000000</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>247.00000000</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>218.80000000</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>243.66000000</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>1019550.75146000</t>
+        </is>
+      </c>
+      <c r="G121" t="n">
+        <v>1590883199999</v>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>238678839.80930440</t>
+        </is>
+      </c>
+      <c r="I121" t="n">
+        <v>341862</v>
+      </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>511425.44765000</t>
+        </is>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>119730479.77167950</t>
+        </is>
+      </c>
+      <c r="L121" t="inlineStr">
+        <is>
+          <t>2020-05-30 08:00:00</t>
+        </is>
+      </c>
+      <c r="M121" t="n">
+        <v>243.6599999999998</v>
+      </c>
+      <c r="N121" t="n">
+        <v>232.1649999999998</v>
+      </c>
+      <c r="O121" t="n">
+        <v>213.9671428571429</v>
+      </c>
+      <c r="P121" t="n">
+        <v>210.4926666666668</v>
+      </c>
+      <c r="Q121" t="n">
+        <v>206.6016666666666</v>
+      </c>
+      <c r="R121" t="n">
+        <v>243.66</v>
+      </c>
+      <c r="S121" t="n">
+        <v>235.4232535943544</v>
+      </c>
+      <c r="T121" t="n">
+        <v>214.2838823190425</v>
+      </c>
+      <c r="U121" t="n">
+        <v>206.8301339683718</v>
+      </c>
+      <c r="V121" t="n">
+        <v>7.453748350670764</v>
+      </c>
+      <c r="W121" t="n">
+        <v>5.009261760258569</v>
+      </c>
+      <c r="X121" t="n">
+        <v>2.444486590412195</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>243.71000000</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>245.39000000</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>229.58000000</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>231.57000000</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>821608.68884000</t>
+        </is>
+      </c>
+      <c r="G122" t="n">
+        <v>1590969599999</v>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>194867426.29418620</t>
+        </is>
+      </c>
+      <c r="I122" t="n">
+        <v>320066</v>
+      </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>381831.06077000</t>
+        </is>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>90551397.67858910</t>
+        </is>
+      </c>
+      <c r="L122" t="inlineStr">
+        <is>
+          <t>2020-05-31 08:00:00</t>
+        </is>
+      </c>
+      <c r="M122" t="n">
+        <v>231.5699999999998</v>
+      </c>
+      <c r="N122" t="n">
+        <v>237.6149999999998</v>
+      </c>
+      <c r="O122" t="n">
+        <v>218.4914285714286</v>
+      </c>
+      <c r="P122" t="n">
+        <v>212.5673333333335</v>
+      </c>
+      <c r="Q122" t="n">
+        <v>207.2533333333333</v>
+      </c>
+      <c r="R122" t="n">
+        <v>231.57</v>
+      </c>
+      <c r="S122" t="n">
+        <v>232.8544178647848</v>
+      </c>
+      <c r="T122" t="n">
+        <v>216.9432850436173</v>
+      </c>
+      <c r="U122" t="n">
+        <v>208.6628821489607</v>
+      </c>
+      <c r="V122" t="n">
+        <v>8.280402894656532</v>
+      </c>
+      <c r="W122" t="n">
+        <v>5.663489987139392</v>
+      </c>
+      <c r="X122" t="n">
+        <v>2.616912907517141</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>231.56000000</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>250.68000000</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>230.66000000</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>248.23000000</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>823816.69936000</t>
+        </is>
+      </c>
+      <c r="G123" t="n">
+        <v>1591055999999</v>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>198791911.84704420</t>
+        </is>
+      </c>
+      <c r="I123" t="n">
+        <v>318497</v>
+      </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>426075.31776000</t>
+        </is>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>102865011.74578850</t>
+        </is>
+      </c>
+      <c r="L123" t="inlineStr">
+        <is>
+          <t>2020-06-01 08:00:00</t>
+        </is>
+      </c>
+      <c r="M123" t="n">
+        <v>248.2299999999998</v>
+      </c>
+      <c r="N123" t="n">
+        <v>239.8999999999999</v>
+      </c>
+      <c r="O123" t="n">
+        <v>224.7885714285714</v>
+      </c>
+      <c r="P123" t="n">
+        <v>215.3160000000001</v>
+      </c>
+      <c r="Q123" t="n">
+        <v>208.3976666666666</v>
+      </c>
+      <c r="R123" t="n">
+        <v>248.23</v>
+      </c>
+      <c r="S123" t="n">
+        <v>243.1048059549283</v>
+      </c>
+      <c r="T123" t="n">
+        <v>221.7566258129183</v>
+      </c>
+      <c r="U123" t="n">
+        <v>211.5940248650075</v>
+      </c>
+      <c r="V123" t="n">
+        <v>10.16260094791073</v>
+      </c>
+      <c r="W123" t="n">
+        <v>6.563312179295012</v>
+      </c>
+      <c r="X123" t="n">
+        <v>3.599288768615721</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>248.23000000</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>253.80000000</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>225.00000000</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>237.71000000</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>955520.91863000</t>
+        </is>
+      </c>
+      <c r="G124" t="n">
+        <v>1591142399999</v>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>230680327.30929150</t>
+        </is>
+      </c>
+      <c r="I124" t="n">
+        <v>355417</v>
+      </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>462682.15945000</t>
+        </is>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>111744961.57192750</t>
+        </is>
+      </c>
+      <c r="L124" t="inlineStr">
+        <is>
+          <t>2020-06-02 08:00:00</t>
+        </is>
+      </c>
+      <c r="M124" t="n">
+        <v>237.7099999999998</v>
+      </c>
+      <c r="N124" t="n">
+        <v>242.9699999999999</v>
+      </c>
+      <c r="O124" t="n">
+        <v>230.0485714285714</v>
+      </c>
+      <c r="P124" t="n">
+        <v>216.8360000000002</v>
+      </c>
+      <c r="Q124" t="n">
+        <v>209.326</v>
+      </c>
+      <c r="R124" t="n">
+        <v>237.71</v>
+      </c>
+      <c r="S124" t="n">
+        <v>239.5082686516428</v>
+      </c>
+      <c r="T124" t="n">
+        <v>224.2109910753948</v>
+      </c>
+      <c r="U124" t="n">
+        <v>213.5286913321422</v>
+      </c>
+      <c r="V124" t="n">
+        <v>10.68229974325263</v>
+      </c>
+      <c r="W124" t="n">
+        <v>7.387109692087526</v>
+      </c>
+      <c r="X124" t="n">
+        <v>3.295190051165102</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>237.71000000</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>245.00000000</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>232.71000000</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>244.52000000</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>502928.13371000</t>
+        </is>
+      </c>
+      <c r="G125" t="n">
+        <v>1591228799999</v>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>120179301.17898640</t>
+        </is>
+      </c>
+      <c r="I125" t="n">
+        <v>213792</v>
+      </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>259904.04578000</t>
+        </is>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>62129185.47385130</t>
+        </is>
+      </c>
+      <c r="L125" t="inlineStr">
+        <is>
+          <t>2020-06-03 08:00:00</t>
+        </is>
+      </c>
+      <c r="M125" t="n">
+        <v>244.5199999999998</v>
+      </c>
+      <c r="N125" t="n">
+        <v>241.1149999999999</v>
+      </c>
+      <c r="O125" t="n">
+        <v>235.2242857142857</v>
+      </c>
+      <c r="P125" t="n">
+        <v>218.8320000000002</v>
+      </c>
+      <c r="Q125" t="n">
+        <v>210.594</v>
+      </c>
+      <c r="R125" t="n">
+        <v>244.52</v>
+      </c>
+      <c r="S125" t="n">
+        <v>242.8494228838809</v>
+      </c>
+      <c r="T125" t="n">
+        <v>227.3354539900239</v>
+      </c>
+      <c r="U125" t="n">
+        <v>215.8245084115693</v>
+      </c>
+      <c r="V125" t="n">
+        <v>11.51094557845457</v>
+      </c>
+      <c r="W125" t="n">
+        <v>8.211876869361728</v>
+      </c>
+      <c r="X125" t="n">
+        <v>3.29906870909284</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>244.54000000</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>246.60000000</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>236.00000000</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>243.21000000</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>669369.33920000</t>
+        </is>
+      </c>
+      <c r="G126" t="n">
+        <v>1591315199999</v>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>162460397.62767410</t>
+        </is>
+      </c>
+      <c r="I126" t="n">
+        <v>253226</v>
+      </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>332175.55769000</t>
+        </is>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>80659519.34918510</t>
+        </is>
+      </c>
+      <c r="L126" t="inlineStr">
+        <is>
+          <t>2020-06-04 08:00:00</t>
+        </is>
+      </c>
+      <c r="M126" t="n">
+        <v>243.2099999999998</v>
+      </c>
+      <c r="N126" t="n">
+        <v>243.8649999999999</v>
+      </c>
+      <c r="O126" t="n">
+        <v>238.51</v>
+      </c>
+      <c r="P126" t="n">
+        <v>221.0473333333335</v>
+      </c>
+      <c r="Q126" t="n">
+        <v>211.858</v>
+      </c>
+      <c r="R126" t="n">
+        <v>243.21</v>
+      </c>
+      <c r="S126" t="n">
+        <v>243.0898076279603</v>
+      </c>
+      <c r="T126" t="n">
+        <v>229.7776918397968</v>
+      </c>
+      <c r="U126" t="n">
+        <v>217.8531980063885</v>
+      </c>
+      <c r="V126" t="n">
+        <v>11.92449383340835</v>
+      </c>
+      <c r="W126" t="n">
+        <v>8.954400262171623</v>
+      </c>
+      <c r="X126" t="n">
+        <v>2.970093571236726</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>243.22000000</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>247.87000000</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>239.14000000</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>240.03000000</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>502547.41103000</t>
+        </is>
+      </c>
+      <c r="G127" t="n">
+        <v>1591401599999</v>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>122084004.51697550</t>
+        </is>
+      </c>
+      <c r="I127" t="n">
+        <v>205337</v>
+      </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>242309.99059000</t>
+        </is>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>58916816.25847680</t>
+        </is>
+      </c>
+      <c r="L127" t="inlineStr">
+        <is>
+          <t>2020-06-05 08:00:00</t>
+        </is>
+      </c>
+      <c r="M127" t="n">
+        <v>240.0299999999998</v>
+      </c>
+      <c r="N127" t="n">
+        <v>241.6199999999999</v>
+      </c>
+      <c r="O127" t="n">
+        <v>241.2757142857143</v>
+      </c>
+      <c r="P127" t="n">
+        <v>223.8000000000002</v>
+      </c>
+      <c r="Q127" t="n">
+        <v>213.2266666666666</v>
+      </c>
+      <c r="R127" t="n">
+        <v>240.03</v>
+      </c>
+      <c r="S127" t="n">
+        <v>241.0499358759868</v>
+      </c>
+      <c r="T127" t="n">
+        <v>231.3549700194286</v>
+      </c>
+      <c r="U127" t="n">
+        <v>219.4960250514532</v>
+      </c>
+      <c r="V127" t="n">
+        <v>11.85894496797545</v>
+      </c>
+      <c r="W127" t="n">
+        <v>9.535309203332744</v>
+      </c>
+      <c r="X127" t="n">
+        <v>2.323635764642702</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>240.04000000</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>244.70000000</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>237.83000000</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>241.94000000</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>389423.07798000</t>
+        </is>
+      </c>
+      <c r="G128" t="n">
+        <v>1591487999999</v>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>93979350.81263390</t>
+        </is>
+      </c>
+      <c r="I128" t="n">
+        <v>161709</v>
+      </c>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t>198723.53956000</t>
+        </is>
+      </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>47973780.54283710</t>
+        </is>
+      </c>
+      <c r="L128" t="inlineStr">
+        <is>
+          <t>2020-06-06 08:00:00</t>
+        </is>
+      </c>
+      <c r="M128" t="n">
+        <v>241.9399999999998</v>
+      </c>
+      <c r="N128" t="n">
+        <v>240.9849999999999</v>
+      </c>
+      <c r="O128" t="n">
+        <v>241.03</v>
+      </c>
+      <c r="P128" t="n">
+        <v>226.1053333333335</v>
+      </c>
+      <c r="Q128" t="n">
+        <v>214.2246666666666</v>
+      </c>
+      <c r="R128" t="n">
+        <v>241.94</v>
+      </c>
+      <c r="S128" t="n">
+        <v>241.6433119586623</v>
+      </c>
+      <c r="T128" t="n">
+        <v>232.9834361712808</v>
+      </c>
+      <c r="U128" t="n">
+        <v>221.1586363323111</v>
+      </c>
+      <c r="V128" t="n">
+        <v>11.82479983896971</v>
+      </c>
+      <c r="W128" t="n">
+        <v>9.993207330460363</v>
+      </c>
+      <c r="X128" t="n">
+        <v>1.831592508509347</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>241.94000000</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>245.37000000</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>234.60000000</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>244.56000000</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>571102.55515000</t>
+        </is>
+      </c>
+      <c r="G129" t="n">
+        <v>1591574399999</v>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>137165732.64761660</t>
+        </is>
+      </c>
+      <c r="I129" t="n">
+        <v>226478</v>
+      </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>285159.65388000</t>
+        </is>
+      </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>68517428.42271850</t>
+        </is>
+      </c>
+      <c r="L129" t="inlineStr">
+        <is>
+          <t>2020-06-07 08:00:00</t>
+        </is>
+      </c>
+      <c r="M129" t="n">
+        <v>244.5599999999998</v>
+      </c>
+      <c r="N129" t="n">
+        <v>243.2499999999999</v>
+      </c>
+      <c r="O129" t="n">
+        <v>242.8857142857143</v>
+      </c>
+      <c r="P129" t="n">
+        <v>228.6360000000002</v>
+      </c>
+      <c r="Q129" t="n">
+        <v>215.333</v>
+      </c>
+      <c r="R129" t="n">
+        <v>244.56</v>
+      </c>
+      <c r="S129" t="n">
+        <v>243.5877706528874</v>
+      </c>
+      <c r="T129" t="n">
+        <v>234.7644459920046</v>
+      </c>
+      <c r="U129" t="n">
+        <v>222.8921620240754</v>
+      </c>
+      <c r="V129" t="n">
+        <v>11.87228396792921</v>
+      </c>
+      <c r="W129" t="n">
+        <v>10.36902265795428</v>
+      </c>
+      <c r="X129" t="n">
+        <v>1.503261309974928</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>244.57000000</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>247.70000000</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>240.59000000</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>246.40000000</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>383116.54719000</t>
+        </is>
+      </c>
+      <c r="G130" t="n">
+        <v>1591660799999</v>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>93355224.96830870</t>
+        </is>
+      </c>
+      <c r="I130" t="n">
+        <v>159981</v>
+      </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t>193451.07601000</t>
+        </is>
+      </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>47159340.96864370</t>
+        </is>
+      </c>
+      <c r="L130" t="inlineStr">
+        <is>
+          <t>2020-06-08 08:00:00</t>
+        </is>
+      </c>
+      <c r="M130" t="n">
+        <v>246.3999999999998</v>
+      </c>
+      <c r="N130" t="n">
+        <v>245.4799999999999</v>
+      </c>
+      <c r="O130" t="n">
+        <v>242.6242857142857</v>
+      </c>
+      <c r="P130" t="n">
+        <v>231.7360000000002</v>
+      </c>
+      <c r="Q130" t="n">
+        <v>216.544</v>
+      </c>
+      <c r="R130" t="n">
+        <v>246.4</v>
+      </c>
+      <c r="S130" t="n">
+        <v>245.4625902176291</v>
+      </c>
+      <c r="T130" t="n">
+        <v>236.5545312247871</v>
+      </c>
+      <c r="U130" t="n">
+        <v>224.6335683197628</v>
+      </c>
+      <c r="V130" t="n">
+        <v>11.92096290502431</v>
+      </c>
+      <c r="W130" t="n">
+        <v>10.67941070736838</v>
+      </c>
+      <c r="X130" t="n">
+        <v>1.241552197655928</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>246.37000000</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>249.82000000</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>238.00000000</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>243.80000000</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>420327.17133000</t>
+        </is>
+      </c>
+      <c r="G131" t="n">
+        <v>1591747199999</v>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>102374504.57389720</t>
+        </is>
+      </c>
+      <c r="I131" t="n">
+        <v>185974</v>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>202641.07177000</t>
+        </is>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>49369436.33086970</t>
+        </is>
+      </c>
+      <c r="L131" t="inlineStr">
+        <is>
+          <t>2020-06-09 08:00:00</t>
+        </is>
+      </c>
+      <c r="M131" t="n">
+        <v>243.7999999999998</v>
+      </c>
+      <c r="N131" t="n">
+        <v>245.0999999999999</v>
+      </c>
+      <c r="O131" t="n">
+        <v>243.4942857142857</v>
+      </c>
+      <c r="P131" t="n">
+        <v>234.3793333333335</v>
+      </c>
+      <c r="Q131" t="n">
+        <v>218.4193333333333</v>
+      </c>
+      <c r="R131" t="n">
+        <v>243.8</v>
+      </c>
+      <c r="S131" t="n">
+        <v>244.3541967392097</v>
+      </c>
+      <c r="T131" t="n">
+        <v>237.6692187290786</v>
+      </c>
+      <c r="U131" t="n">
+        <v>226.0533681412496</v>
+      </c>
+      <c r="V131" t="n">
+        <v>11.61585058782899</v>
+      </c>
+      <c r="W131" t="n">
+        <v>10.86669868346055</v>
+      </c>
+      <c r="X131" t="n">
+        <v>0.7491519043684356</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>243.79000000</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>244.88000000</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>242.20000000</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>243.26000000</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>143398.51855000</t>
+        </is>
+      </c>
+      <c r="G132" t="n">
+        <v>1591833599999</v>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>34922579.34856620</t>
+        </is>
+      </c>
+      <c r="I132" t="n">
+        <v>70298</v>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>67192.29042000</t>
+        </is>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>16365116.18958130</t>
+        </is>
+      </c>
+      <c r="L132" t="inlineStr">
+        <is>
+          <t>2020-06-10 08:00:00</t>
+        </is>
+      </c>
+      <c r="M132" t="n">
+        <v>243.2599999999998</v>
+      </c>
+      <c r="N132" t="n">
+        <v>243.5299999999999</v>
+      </c>
+      <c r="O132" t="n">
+        <v>243.3142857142857</v>
+      </c>
+      <c r="P132" t="n">
+        <v>237.2040000000002</v>
+      </c>
+      <c r="Q132" t="n">
+        <v>220.337</v>
+      </c>
+      <c r="R132" t="n">
+        <v>243.26</v>
+      </c>
+      <c r="S132" t="n">
+        <v>243.6247322464032</v>
+      </c>
+      <c r="T132" t="n">
+        <v>238.5293389248744</v>
+      </c>
+      <c r="U132" t="n">
+        <v>227.3279867814382</v>
+      </c>
+      <c r="V132" t="n">
+        <v>11.20135214343622</v>
+      </c>
+      <c r="W132" t="n">
+        <v>10.9336293754557</v>
+      </c>
+      <c r="X132" t="n">
+        <v>0.2677227679805245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the send mail condition
</commit_message>
<xml_diff>
--- a/Data/binance_ETHUSDT_data.xlsx
+++ b/Data/binance_ETHUSDT_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X132"/>
+  <dimension ref="A1:X134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12354,22 +12354,22 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>244.88000000</t>
+          <t>250.28000000</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>242.20000000</t>
+          <t>242.00000000</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>243.26000000</t>
+          <t>247.78000000</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>143398.51855000</t>
+          <t>431285.61715000</t>
         </is>
       </c>
       <c r="G132" t="n">
@@ -12377,20 +12377,20 @@
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>34922579.34856620</t>
+          <t>105797248.24742570</t>
         </is>
       </c>
       <c r="I132" t="n">
-        <v>70298</v>
+        <v>185330</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
-          <t>67192.29042000</t>
+          <t>221305.11120000</t>
         </is>
       </c>
       <c r="K132" t="inlineStr">
         <is>
-          <t>16365116.18958130</t>
+          <t>54322143.50039510</t>
         </is>
       </c>
       <c r="L132" t="inlineStr">
@@ -12399,40 +12399,224 @@
         </is>
       </c>
       <c r="M132" t="n">
-        <v>243.2599999999998</v>
+        <v>247.7799999999998</v>
       </c>
       <c r="N132" t="n">
-        <v>243.5299999999999</v>
+        <v>245.7899999999999</v>
       </c>
       <c r="O132" t="n">
-        <v>243.3142857142857</v>
+        <v>243.96</v>
       </c>
       <c r="P132" t="n">
-        <v>237.2040000000002</v>
+        <v>237.5053333333335</v>
       </c>
       <c r="Q132" t="n">
-        <v>220.337</v>
+        <v>220.4876666666666</v>
       </c>
       <c r="R132" t="n">
-        <v>243.26</v>
+        <v>247.78</v>
       </c>
       <c r="S132" t="n">
-        <v>243.6247322464032</v>
+        <v>246.6380655797366</v>
       </c>
       <c r="T132" t="n">
-        <v>238.5293389248744</v>
+        <v>239.2247235404768</v>
       </c>
       <c r="U132" t="n">
-        <v>227.3279867814382</v>
+        <v>227.662815602148</v>
       </c>
       <c r="V132" t="n">
-        <v>11.20135214343622</v>
+        <v>11.56190793832886</v>
       </c>
       <c r="W132" t="n">
-        <v>10.9336293754557</v>
+        <v>11.00574053443424</v>
       </c>
       <c r="X132" t="n">
-        <v>0.2677227679805245</v>
+        <v>0.5561674038946158</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>247.78000000</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>250.09000000</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>226.20000000</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>230.51000000</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>816456.89161000</t>
+        </is>
+      </c>
+      <c r="G133" t="n">
+        <v>1591919999999</v>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>195063781.27644910</t>
+        </is>
+      </c>
+      <c r="I133" t="n">
+        <v>312655</v>
+      </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>373492.34304000</t>
+        </is>
+      </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>89279896.48515260</t>
+        </is>
+      </c>
+      <c r="L133" t="inlineStr">
+        <is>
+          <t>2020-06-11 08:00:00</t>
+        </is>
+      </c>
+      <c r="M133" t="n">
+        <v>230.5099999999998</v>
+      </c>
+      <c r="N133" t="n">
+        <v>239.1449999999999</v>
+      </c>
+      <c r="O133" t="n">
+        <v>242.1457142857143</v>
+      </c>
+      <c r="P133" t="n">
+        <v>238.9866666666668</v>
+      </c>
+      <c r="Q133" t="n">
+        <v>221.846</v>
+      </c>
+      <c r="R133" t="n">
+        <v>230.51</v>
+      </c>
+      <c r="S133" t="n">
+        <v>235.8860218599122</v>
+      </c>
+      <c r="T133" t="n">
+        <v>237.8839968415866</v>
+      </c>
+      <c r="U133" t="n">
+        <v>227.8737263190247</v>
+      </c>
+      <c r="V133" t="n">
+        <v>10.01027052256188</v>
+      </c>
+      <c r="W133" t="n">
+        <v>10.80664653205974</v>
+      </c>
+      <c r="X133" t="n">
+        <v>-0.7963760094978554</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>230.46000000</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>239.38000000</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>228.19000000</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>235.22000000</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>397549.31654000</t>
+        </is>
+      </c>
+      <c r="G134" t="n">
+        <v>1592006399999</v>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>93464813.52779320</t>
+        </is>
+      </c>
+      <c r="I134" t="n">
+        <v>154895</v>
+      </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>199267.27950000</t>
+        </is>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>46876827.74583840</t>
+        </is>
+      </c>
+      <c r="L134" t="inlineStr">
+        <is>
+          <t>2020-06-12 08:00:00</t>
+        </is>
+      </c>
+      <c r="M134" t="n">
+        <v>235.2199999999998</v>
+      </c>
+      <c r="N134" t="n">
+        <v>232.8649999999999</v>
+      </c>
+      <c r="O134" t="n">
+        <v>241.4585714285714</v>
+      </c>
+      <c r="P134" t="n">
+        <v>239.9873333333335</v>
+      </c>
+      <c r="Q134" t="n">
+        <v>223.034</v>
+      </c>
+      <c r="R134" t="n">
+        <v>235.22</v>
+      </c>
+      <c r="S134" t="n">
+        <v>235.4420072866374</v>
+      </c>
+      <c r="T134" t="n">
+        <v>237.4741511735583</v>
+      </c>
+      <c r="U134" t="n">
+        <v>228.4179142557757</v>
+      </c>
+      <c r="V134" t="n">
+        <v>9.05623691778257</v>
+      </c>
+      <c r="W134" t="n">
+        <v>10.45656460920426</v>
+      </c>
+      <c r="X134" t="n">
+        <v>-1.40032769142169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update with Position Function
</commit_message>
<xml_diff>
--- a/Data/binance_ETHUSDT_data.xlsx
+++ b/Data/binance_ETHUSDT_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X157"/>
+  <dimension ref="A1:X165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14654,7 +14654,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>385.59000000</t>
+          <t>390.00000000</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -14664,12 +14664,12 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>381.48000000</t>
+          <t>387.88000000</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>560508.44244000</t>
+          <t>752954.37114000</t>
         </is>
       </c>
       <c r="G157" t="n">
@@ -14677,20 +14677,20 @@
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>212301131.56568030</t>
+          <t>286291773.96848450</t>
         </is>
       </c>
       <c r="I157" t="n">
-        <v>203841</v>
+        <v>280412</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
-          <t>266829.98441000</t>
+          <t>366506.41600000</t>
         </is>
       </c>
       <c r="K157" t="inlineStr">
         <is>
-          <t>101112597.15977730</t>
+          <t>139475874.91715260</t>
         </is>
       </c>
       <c r="L157" t="inlineStr">
@@ -14699,40 +14699,776 @@
         </is>
       </c>
       <c r="M157" t="n">
-        <v>381.4799999999996</v>
+        <v>387.8799999999997</v>
       </c>
       <c r="N157" t="n">
-        <v>382.2499999999999</v>
+        <v>385.4499999999998</v>
       </c>
       <c r="O157" t="n">
-        <v>386.4971428571428</v>
+        <v>387.4114285714285</v>
       </c>
       <c r="P157" t="n">
-        <v>393.4293333333333</v>
+        <v>393.8559999999999</v>
       </c>
       <c r="Q157" t="n">
-        <v>380.4383333333333</v>
+        <v>380.6516666666666</v>
       </c>
       <c r="R157" t="n">
-        <v>381.48</v>
+        <v>387.88</v>
       </c>
       <c r="S157" t="n">
-        <v>383.1094939056179</v>
+        <v>387.3761605722846</v>
       </c>
       <c r="T157" t="n">
-        <v>388.3603791275044</v>
+        <v>389.3449945121245</v>
       </c>
       <c r="U157" t="n">
-        <v>384.0820371241896</v>
+        <v>384.5561140938933</v>
       </c>
       <c r="V157" t="n">
-        <v>4.278342003314776</v>
+        <v>4.788880418231201</v>
       </c>
       <c r="W157" t="n">
-        <v>6.631430181933227</v>
+        <v>6.733537864916512</v>
       </c>
       <c r="X157" t="n">
-        <v>-2.35308817861845</v>
+        <v>-1.94465744668531</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>387.88000000</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>408.39000000</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>376.47000000</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>402.49000000</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>1157064.35076000</t>
+        </is>
+      </c>
+      <c r="G158" t="n">
+        <v>1604534399999</v>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>454481208.40200980</t>
+        </is>
+      </c>
+      <c r="I158" t="n">
+        <v>392310</v>
+      </c>
+      <c r="J158" t="inlineStr">
+        <is>
+          <t>600951.59602000</t>
+        </is>
+      </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>236190448.28833480</t>
+        </is>
+      </c>
+      <c r="L158" t="inlineStr">
+        <is>
+          <t>2020-11-04 08:00:00</t>
+        </is>
+      </c>
+      <c r="M158" t="n">
+        <v>402.4899999999997</v>
+      </c>
+      <c r="N158" t="n">
+        <v>395.1849999999998</v>
+      </c>
+      <c r="O158" t="n">
+        <v>389.4485714285714</v>
+      </c>
+      <c r="P158" t="n">
+        <v>396.1206666666666</v>
+      </c>
+      <c r="Q158" t="n">
+        <v>382.2806666666665</v>
+      </c>
+      <c r="R158" t="n">
+        <v>402.49</v>
+      </c>
+      <c r="S158" t="n">
+        <v>397.4520535240949</v>
+      </c>
+      <c r="T158" t="n">
+        <v>391.367303048729</v>
+      </c>
+      <c r="U158" t="n">
+        <v>385.8845575999398</v>
+      </c>
+      <c r="V158" t="n">
+        <v>5.48274544878916</v>
+      </c>
+      <c r="W158" t="n">
+        <v>6.483379381691043</v>
+      </c>
+      <c r="X158" t="n">
+        <v>-1.000633932901883</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>402.50000000</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>420.40000000</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>396.14000000</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>416.69000000</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>1475139.77342000</t>
+        </is>
+      </c>
+      <c r="G159" t="n">
+        <v>1604620799999</v>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>601591250.40124900</t>
+        </is>
+      </c>
+      <c r="I159" t="n">
+        <v>513574</v>
+      </c>
+      <c r="J159" t="inlineStr">
+        <is>
+          <t>733696.12776000</t>
+        </is>
+      </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>299466668.01144860</t>
+        </is>
+      </c>
+      <c r="L159" t="inlineStr">
+        <is>
+          <t>2020-11-05 08:00:00</t>
+        </is>
+      </c>
+      <c r="M159" t="n">
+        <v>416.6899999999996</v>
+      </c>
+      <c r="N159" t="n">
+        <v>409.5899999999999</v>
+      </c>
+      <c r="O159" t="n">
+        <v>393.6714285714285</v>
+      </c>
+      <c r="P159" t="n">
+        <v>397.8746666666666</v>
+      </c>
+      <c r="Q159" t="n">
+        <v>384.8119999999999</v>
+      </c>
+      <c r="R159" t="n">
+        <v>416.69</v>
+      </c>
+      <c r="S159" t="n">
+        <v>410.2773511746983</v>
+      </c>
+      <c r="T159" t="n">
+        <v>395.2631025797072</v>
+      </c>
+      <c r="U159" t="n">
+        <v>388.1664541714699</v>
+      </c>
+      <c r="V159" t="n">
+        <v>7.096648408237286</v>
+      </c>
+      <c r="W159" t="n">
+        <v>6.606033187000292</v>
+      </c>
+      <c r="X159" t="n">
+        <v>0.4906152212369941</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>416.73000000</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>458.27000000</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>414.76000000</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>455.91000000</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>1682440.96026000</t>
+        </is>
+      </c>
+      <c r="G160" t="n">
+        <v>1604707199999</v>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>736015135.62721030</t>
+        </is>
+      </c>
+      <c r="I160" t="n">
+        <v>666505</v>
+      </c>
+      <c r="J160" t="inlineStr">
+        <is>
+          <t>883105.68936000</t>
+        </is>
+      </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>386541087.43089730</t>
+        </is>
+      </c>
+      <c r="L160" t="inlineStr">
+        <is>
+          <t>2020-11-06 08:00:00</t>
+        </is>
+      </c>
+      <c r="M160" t="n">
+        <v>455.9099999999997</v>
+      </c>
+      <c r="N160" t="n">
+        <v>436.2999999999998</v>
+      </c>
+      <c r="O160" t="n">
+        <v>404.16</v>
+      </c>
+      <c r="P160" t="n">
+        <v>400.67</v>
+      </c>
+      <c r="Q160" t="n">
+        <v>388.6229999999999</v>
+      </c>
+      <c r="R160" t="n">
+        <v>455.91</v>
+      </c>
+      <c r="S160" t="n">
+        <v>440.6991170582328</v>
+      </c>
+      <c r="T160" t="n">
+        <v>404.5933944905486</v>
+      </c>
+      <c r="U160" t="n">
+        <v>393.1845189341669</v>
+      </c>
+      <c r="V160" t="n">
+        <v>11.4088755563817</v>
+      </c>
+      <c r="W160" t="n">
+        <v>7.566601660876574</v>
+      </c>
+      <c r="X160" t="n">
+        <v>3.842273895505127</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>455.91000000</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>468.28000000</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>424.14000000</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>435.21000000</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>1653416.59610000</t>
+        </is>
+      </c>
+      <c r="G161" t="n">
+        <v>1604793599999</v>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>743871175.78212340</t>
+        </is>
+      </c>
+      <c r="I161" t="n">
+        <v>674858</v>
+      </c>
+      <c r="J161" t="inlineStr">
+        <is>
+          <t>831369.37192000</t>
+        </is>
+      </c>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>374507765.44837650</t>
+        </is>
+      </c>
+      <c r="L161" t="inlineStr">
+        <is>
+          <t>2020-11-07 08:00:00</t>
+        </is>
+      </c>
+      <c r="M161" t="n">
+        <v>435.2099999999996</v>
+      </c>
+      <c r="N161" t="n">
+        <v>445.5599999999998</v>
+      </c>
+      <c r="O161" t="n">
+        <v>411.1242857142857</v>
+      </c>
+      <c r="P161" t="n">
+        <v>402.41</v>
+      </c>
+      <c r="Q161" t="n">
+        <v>391.4316666666665</v>
+      </c>
+      <c r="R161" t="n">
+        <v>435.21</v>
+      </c>
+      <c r="S161" t="n">
+        <v>437.0397056860776</v>
+      </c>
+      <c r="T161" t="n">
+        <v>409.3036414920143</v>
+      </c>
+      <c r="U161" t="n">
+        <v>396.2975315075429</v>
+      </c>
+      <c r="V161" t="n">
+        <v>13.00610998447144</v>
+      </c>
+      <c r="W161" t="n">
+        <v>8.654503325595547</v>
+      </c>
+      <c r="X161" t="n">
+        <v>4.351606658875889</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>435.20000000</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>460.10000000</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>431.99000000</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>454.30000000</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>840908.46841000</t>
+        </is>
+      </c>
+      <c r="G162" t="n">
+        <v>1604879999999</v>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>375679148.23503960</t>
+        </is>
+      </c>
+      <c r="I162" t="n">
+        <v>354341</v>
+      </c>
+      <c r="J162" t="inlineStr">
+        <is>
+          <t>424300.36519000</t>
+        </is>
+      </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>189644075.40081470</t>
+        </is>
+      </c>
+      <c r="L162" t="inlineStr">
+        <is>
+          <t>2020-11-08 08:00:00</t>
+        </is>
+      </c>
+      <c r="M162" t="n">
+        <v>454.2999999999997</v>
+      </c>
+      <c r="N162" t="n">
+        <v>444.7549999999998</v>
+      </c>
+      <c r="O162" t="n">
+        <v>419.3571428571428</v>
+      </c>
+      <c r="P162" t="n">
+        <v>405.2206666666667</v>
+      </c>
+      <c r="Q162" t="n">
+        <v>394.4076666666664</v>
+      </c>
+      <c r="R162" t="n">
+        <v>454.3</v>
+      </c>
+      <c r="S162" t="n">
+        <v>448.5465685620259</v>
+      </c>
+      <c r="T162" t="n">
+        <v>416.2261581855651</v>
+      </c>
+      <c r="U162" t="n">
+        <v>400.5940285154788</v>
+      </c>
+      <c r="V162" t="n">
+        <v>15.63212967008627</v>
+      </c>
+      <c r="W162" t="n">
+        <v>10.05002859449369</v>
+      </c>
+      <c r="X162" t="n">
+        <v>5.582101075592579</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>454.29000000</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>459.10000000</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>433.09000000</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>444.32000000</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>1099213.24641000</t>
+        </is>
+      </c>
+      <c r="G163" t="n">
+        <v>1604966399999</v>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>491928164.98124340</t>
+        </is>
+      </c>
+      <c r="I163" t="n">
+        <v>469947</v>
+      </c>
+      <c r="J163" t="inlineStr">
+        <is>
+          <t>523180.45111000</t>
+        </is>
+      </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>234223108.98942740</t>
+        </is>
+      </c>
+      <c r="L163" t="inlineStr">
+        <is>
+          <t>2020-11-09 08:00:00</t>
+        </is>
+      </c>
+      <c r="M163" t="n">
+        <v>444.3199999999997</v>
+      </c>
+      <c r="N163" t="n">
+        <v>449.3099999999997</v>
+      </c>
+      <c r="O163" t="n">
+        <v>428.1142857142858</v>
+      </c>
+      <c r="P163" t="n">
+        <v>407.7846666666666</v>
+      </c>
+      <c r="Q163" t="n">
+        <v>396.8676666666664</v>
+      </c>
+      <c r="R163" t="n">
+        <v>444.32</v>
+      </c>
+      <c r="S163" t="n">
+        <v>445.728856187342</v>
+      </c>
+      <c r="T163" t="n">
+        <v>420.5482876954858</v>
+      </c>
+      <c r="U163" t="n">
+        <v>403.8330018330985</v>
+      </c>
+      <c r="V163" t="n">
+        <v>16.71528586238725</v>
+      </c>
+      <c r="W163" t="n">
+        <v>11.3830800480724</v>
+      </c>
+      <c r="X163" t="n">
+        <v>5.332205814314843</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>444.32000000</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>455.00000000</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>438.70000000</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>450.34000000</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>866872.41108000</t>
+        </is>
+      </c>
+      <c r="G164" t="n">
+        <v>1605052799999</v>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>388190148.20789510</t>
+        </is>
+      </c>
+      <c r="I164" t="n">
+        <v>384228</v>
+      </c>
+      <c r="J164" t="inlineStr">
+        <is>
+          <t>437244.02871000</t>
+        </is>
+      </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>195856348.18969540</t>
+        </is>
+      </c>
+      <c r="L164" t="inlineStr">
+        <is>
+          <t>2020-11-10 08:00:00</t>
+        </is>
+      </c>
+      <c r="M164" t="n">
+        <v>450.3399999999996</v>
+      </c>
+      <c r="N164" t="n">
+        <v>447.3299999999997</v>
+      </c>
+      <c r="O164" t="n">
+        <v>437.0371428571429</v>
+      </c>
+      <c r="P164" t="n">
+        <v>411.6393333333334</v>
+      </c>
+      <c r="Q164" t="n">
+        <v>399.4069999999998</v>
+      </c>
+      <c r="R164" t="n">
+        <v>450.34</v>
+      </c>
+      <c r="S164" t="n">
+        <v>448.8029520624473</v>
+      </c>
+      <c r="T164" t="n">
+        <v>425.1316280500333</v>
+      </c>
+      <c r="U164" t="n">
+        <v>407.2779769378895</v>
+      </c>
+      <c r="V164" t="n">
+        <v>17.85365111214378</v>
+      </c>
+      <c r="W164" t="n">
+        <v>12.67719426088668</v>
+      </c>
+      <c r="X164" t="n">
+        <v>5.176456851257099</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>450.34000000</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>474.00000000</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>449.28000000</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>469.23000000</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>872086.75803000</t>
+        </is>
+      </c>
+      <c r="G165" t="n">
+        <v>1605139199999</v>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>402974529.15965530</t>
+        </is>
+      </c>
+      <c r="I165" t="n">
+        <v>392598</v>
+      </c>
+      <c r="J165" t="inlineStr">
+        <is>
+          <t>461768.48127000</t>
+        </is>
+      </c>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>213396558.17390210</t>
+        </is>
+      </c>
+      <c r="L165" t="inlineStr">
+        <is>
+          <t>2020-11-11 08:00:00</t>
+        </is>
+      </c>
+      <c r="M165" t="n">
+        <v>469.2299999999997</v>
+      </c>
+      <c r="N165" t="n">
+        <v>459.7849999999997</v>
+      </c>
+      <c r="O165" t="n">
+        <v>446.5714285714286</v>
+      </c>
+      <c r="P165" t="n">
+        <v>416.0246666666666</v>
+      </c>
+      <c r="Q165" t="n">
+        <v>402.1643333333331</v>
+      </c>
+      <c r="R165" t="n">
+        <v>469.23</v>
+      </c>
+      <c r="S165" t="n">
+        <v>462.4209840208158</v>
+      </c>
+      <c r="T165" t="n">
+        <v>431.9159929654214</v>
+      </c>
+      <c r="U165" t="n">
+        <v>411.8670308267658</v>
+      </c>
+      <c r="V165" t="n">
+        <v>20.04896213865561</v>
+      </c>
+      <c r="W165" t="n">
+        <v>14.15154783644047</v>
+      </c>
+      <c r="X165" t="n">
+        <v>5.89741430221514</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2020-11-15 - Update for Retreive Position Of selling or buying
</commit_message>
<xml_diff>
--- a/Data/binance_ETHUSDT_data.xlsx
+++ b/Data/binance_ETHUSDT_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X165"/>
+  <dimension ref="A1:X169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15390,7 +15390,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>474.00000000</t>
+          <t>476.25000000</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
@@ -15400,12 +15400,12 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>469.23000000</t>
+          <t>463.09000000</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>872086.75803000</t>
+          <t>1205782.84262000</t>
         </is>
       </c>
       <c r="G165" t="n">
@@ -15413,20 +15413,20 @@
       </c>
       <c r="H165" t="inlineStr">
         <is>
-          <t>402974529.15965530</t>
+          <t>559228791.89035090</t>
         </is>
       </c>
       <c r="I165" t="n">
-        <v>392598</v>
+        <v>560360</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
-          <t>461768.48127000</t>
+          <t>626267.49881000</t>
         </is>
       </c>
       <c r="K165" t="inlineStr">
         <is>
-          <t>213396558.17390210</t>
+          <t>290487786.95615110</t>
         </is>
       </c>
       <c r="L165" t="inlineStr">
@@ -15435,40 +15435,408 @@
         </is>
       </c>
       <c r="M165" t="n">
-        <v>469.2299999999997</v>
+        <v>463.0899999999996</v>
       </c>
       <c r="N165" t="n">
-        <v>459.7849999999997</v>
+        <v>456.7149999999997</v>
       </c>
       <c r="O165" t="n">
-        <v>446.5714285714286</v>
+        <v>445.6942857142858</v>
       </c>
       <c r="P165" t="n">
-        <v>416.0246666666666</v>
+        <v>415.6153333333334</v>
       </c>
       <c r="Q165" t="n">
-        <v>402.1643333333331</v>
+        <v>401.9596666666665</v>
       </c>
       <c r="R165" t="n">
-        <v>469.23</v>
+        <v>463.09</v>
       </c>
       <c r="S165" t="n">
-        <v>462.4209840208158</v>
+        <v>458.3276506874824</v>
       </c>
       <c r="T165" t="n">
-        <v>431.9159929654214</v>
+        <v>430.9713775808049</v>
       </c>
       <c r="U165" t="n">
-        <v>411.8670308267658</v>
+        <v>411.4122145110911</v>
       </c>
       <c r="V165" t="n">
-        <v>20.04896213865561</v>
+        <v>19.55916306971375</v>
       </c>
       <c r="W165" t="n">
-        <v>14.15154783644047</v>
+        <v>14.0535880226521</v>
       </c>
       <c r="X165" t="n">
-        <v>5.89741430221514</v>
+        <v>5.505575047061649</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>463.09000000</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>470.00000000</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>451.20000000</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>462.39000000</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>990776.62912000</t>
+        </is>
+      </c>
+      <c r="G166" t="n">
+        <v>1605225599999</v>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>455971309.21685460</t>
+        </is>
+      </c>
+      <c r="I166" t="n">
+        <v>411840</v>
+      </c>
+      <c r="J166" t="inlineStr">
+        <is>
+          <t>471577.98126000</t>
+        </is>
+      </c>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>217115755.31874190</t>
+        </is>
+      </c>
+      <c r="L166" t="inlineStr">
+        <is>
+          <t>2020-11-12 08:00:00</t>
+        </is>
+      </c>
+      <c r="M166" t="n">
+        <v>462.3899999999996</v>
+      </c>
+      <c r="N166" t="n">
+        <v>462.7399999999997</v>
+      </c>
+      <c r="O166" t="n">
+        <v>452.2228571428572</v>
+      </c>
+      <c r="P166" t="n">
+        <v>420.5593333333334</v>
+      </c>
+      <c r="Q166" t="n">
+        <v>404.6713333333331</v>
+      </c>
+      <c r="R166" t="n">
+        <v>462.39</v>
+      </c>
+      <c r="S166" t="n">
+        <v>461.0358835624941</v>
+      </c>
+      <c r="T166" t="n">
+        <v>435.8050117991477</v>
+      </c>
+      <c r="U166" t="n">
+        <v>415.1883583074846</v>
+      </c>
+      <c r="V166" t="n">
+        <v>20.61665349166316</v>
+      </c>
+      <c r="W166" t="n">
+        <v>15.36620111645431</v>
+      </c>
+      <c r="X166" t="n">
+        <v>5.250452375208846</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>462.48000000</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>478.01000000</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>457.12000000</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>476.43000000</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>976665.09752000</t>
+        </is>
+      </c>
+      <c r="G167" t="n">
+        <v>1605311999999</v>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>456232937.20613030</t>
+        </is>
+      </c>
+      <c r="I167" t="n">
+        <v>427363</v>
+      </c>
+      <c r="J167" t="inlineStr">
+        <is>
+          <t>509344.22798000</t>
+        </is>
+      </c>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>238031863.05169850</t>
+        </is>
+      </c>
+      <c r="L167" t="inlineStr">
+        <is>
+          <t>2020-11-13 08:00:00</t>
+        </is>
+      </c>
+      <c r="M167" t="n">
+        <v>476.4299999999996</v>
+      </c>
+      <c r="N167" t="n">
+        <v>469.4099999999997</v>
+      </c>
+      <c r="O167" t="n">
+        <v>455.1542857142858</v>
+      </c>
+      <c r="P167" t="n">
+        <v>426.5126666666667</v>
+      </c>
+      <c r="Q167" t="n">
+        <v>407.9293333333331</v>
+      </c>
+      <c r="R167" t="n">
+        <v>476.43</v>
+      </c>
+      <c r="S167" t="n">
+        <v>471.2986278541647</v>
+      </c>
+      <c r="T167" t="n">
+        <v>442.0550099838998</v>
+      </c>
+      <c r="U167" t="n">
+        <v>419.7247890448951</v>
+      </c>
+      <c r="V167" t="n">
+        <v>22.33022093900473</v>
+      </c>
+      <c r="W167" t="n">
+        <v>16.7590050809644</v>
+      </c>
+      <c r="X167" t="n">
+        <v>5.571215858040336</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>476.42000000</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>477.47000000</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>452.00000000</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>460.89000000</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>735252.78540000</t>
+        </is>
+      </c>
+      <c r="G168" t="n">
+        <v>1605398399999</v>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>340142257.19369760</t>
+        </is>
+      </c>
+      <c r="I168" t="n">
+        <v>350772</v>
+      </c>
+      <c r="J168" t="inlineStr">
+        <is>
+          <t>347000.03929000</t>
+        </is>
+      </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>160634962.00481430</t>
+        </is>
+      </c>
+      <c r="L168" t="inlineStr">
+        <is>
+          <t>2020-11-14 08:00:00</t>
+        </is>
+      </c>
+      <c r="M168" t="n">
+        <v>460.8899999999996</v>
+      </c>
+      <c r="N168" t="n">
+        <v>468.6599999999998</v>
+      </c>
+      <c r="O168" t="n">
+        <v>458.8228571428572</v>
+      </c>
+      <c r="P168" t="n">
+        <v>431.7393333333335</v>
+      </c>
+      <c r="Q168" t="n">
+        <v>410.7043333333331</v>
+      </c>
+      <c r="R168" t="n">
+        <v>460.89</v>
+      </c>
+      <c r="S168" t="n">
+        <v>464.3595426180549</v>
+      </c>
+      <c r="T168" t="n">
+        <v>444.9527007556097</v>
+      </c>
+      <c r="U168" t="n">
+        <v>422.7740719183204</v>
+      </c>
+      <c r="V168" t="n">
+        <v>22.17862883728935</v>
+      </c>
+      <c r="W168" t="n">
+        <v>17.84292983222939</v>
+      </c>
+      <c r="X168" t="n">
+        <v>4.335699005059965</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>460.90000000</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>462.89000000</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>456.51000000</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>461.24000000</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>128673.84301000</t>
+        </is>
+      </c>
+      <c r="G169" t="n">
+        <v>1605484799999</v>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>59155584.09075830</t>
+        </is>
+      </c>
+      <c r="I169" t="n">
+        <v>66228</v>
+      </c>
+      <c r="J169" t="inlineStr">
+        <is>
+          <t>67273.91394000</t>
+        </is>
+      </c>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>30926653.60773300</t>
+        </is>
+      </c>
+      <c r="L169" t="inlineStr">
+        <is>
+          <t>2020-11-15 08:00:00</t>
+        </is>
+      </c>
+      <c r="M169" t="n">
+        <v>461.2399999999997</v>
+      </c>
+      <c r="N169" t="n">
+        <v>461.0649999999997</v>
+      </c>
+      <c r="O169" t="n">
+        <v>459.8142857142857</v>
+      </c>
+      <c r="P169" t="n">
+        <v>436.7246666666668</v>
+      </c>
+      <c r="Q169" t="n">
+        <v>413.8956666666664</v>
+      </c>
+      <c r="R169" t="n">
+        <v>461.24</v>
+      </c>
+      <c r="S169" t="n">
+        <v>462.2798475393517</v>
+      </c>
+      <c r="T169" t="n">
+        <v>447.4584391009021</v>
+      </c>
+      <c r="U169" t="n">
+        <v>425.6234068355566</v>
+      </c>
+      <c r="V169" t="n">
+        <v>21.83503226534543</v>
+      </c>
+      <c r="W169" t="n">
+        <v>18.6413503188526</v>
+      </c>
+      <c r="X169" t="n">
+        <v>3.193681946492834</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the Package for import retreive_posiiton
</commit_message>
<xml_diff>
--- a/Data/binance_ETHUSDT_data.xlsx
+++ b/Data/binance_ETHUSDT_data.xlsx
@@ -15768,12 +15768,12 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>460.36000000</t>
+          <t>461.46000000</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>134457.64858000</t>
+          <t>141103.73194000</t>
         </is>
       </c>
       <c r="G169" t="n">
@@ -15781,20 +15781,20 @@
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>61818632.91413330</t>
+          <t>64881689.45175570</t>
         </is>
       </c>
       <c r="I169" t="n">
-        <v>69386</v>
+        <v>72821</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
-          <t>70194.88217000</t>
+          <t>73340.76590000</t>
         </is>
       </c>
       <c r="K169" t="inlineStr">
         <is>
-          <t>32271461.32013870</t>
+          <t>33721369.83236720</t>
         </is>
       </c>
       <c r="L169" t="inlineStr">
@@ -15803,40 +15803,40 @@
         </is>
       </c>
       <c r="M169" t="n">
-        <v>460.3599999999996</v>
+        <v>461.4599999999996</v>
       </c>
       <c r="N169" t="n">
-        <v>460.6249999999998</v>
+        <v>461.1749999999997</v>
       </c>
       <c r="O169" t="n">
-        <v>459.6885714285714</v>
+        <v>459.8457142857143</v>
       </c>
       <c r="P169" t="n">
-        <v>436.6660000000001</v>
+        <v>436.7393333333335</v>
       </c>
       <c r="Q169" t="n">
-        <v>413.8663333333331</v>
+        <v>413.9029999999997</v>
       </c>
       <c r="R169" t="n">
-        <v>460.36</v>
+        <v>461.46</v>
       </c>
       <c r="S169" t="n">
-        <v>461.693180872685</v>
+        <v>462.4265142060183</v>
       </c>
       <c r="T169" t="n">
-        <v>447.3230544855174</v>
+        <v>447.4922852547483</v>
       </c>
       <c r="U169" t="n">
-        <v>425.5582214922616</v>
+        <v>425.6397031713804</v>
       </c>
       <c r="V169" t="n">
-        <v>21.76483299325588</v>
+        <v>21.85258208336791</v>
       </c>
       <c r="W169" t="n">
-        <v>18.62731046443469</v>
+        <v>18.64486028245709</v>
       </c>
       <c r="X169" t="n">
-        <v>3.137522528821194</v>
+        <v>3.207721800910814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>